<commit_message>
Realization of OTP is now taxed as salary
</commit_message>
<xml_diff>
--- a/tests/Feature/config/salary-otp_tenpercent.xlsx
+++ b/tests/Feature/config/salary-otp_tenpercent.xlsx
@@ -309,64 +309,64 @@
 </t>
   </si>
   <si>
-    <t>OTP fra 2038, 1|20 av formuentransfered 510962 with 112412 (tax) to income.2038.income.amount  transfer 510962 (Division: 10219235/20=510962 rewritten rule: 1|19) to income.2038.income.amount  Asset rule:1|20 Division: 10219235/20=510962 rewritten rule: 1|19</t>
+    <t>OTP fra 2038, 1|20 av formuentransfered 510962 with 180701 (tax) to income.2038.income.amount  transfer 510962 (Division: 10219235/20=510962 rewritten rule: 1|19) to income.2038.income.amount  Asset rule:1|20 Division: 10219235/20=510962 rewritten rule: 1|19</t>
   </si>
   <si>
-    <t>transfered 562058 with 123653 (tax) to income.2039.income.amount  transfer 562058 (Division: 10679100/19=562058 rewritten rule: 1|18) to income.2039.income.amount  Asset rule:1|19 Division: 10679100/19=562058 rewritten rule: 1|18</t>
+    <t>transfered 562058 with 199811 (tax) to income.2039.income.amount  transfer 562058 (Division: 10679100/19=562058 rewritten rule: 1|18) to income.2039.income.amount  Asset rule:1|19 Division: 10679100/19=562058 rewritten rule: 1|18</t>
   </si>
   <si>
-    <t>transfered 618264 with 136018 (tax) to income.2040.income.amount  transfer 618264 (Division: 11128746/18=618264 rewritten rule: 1|17) to income.2040.income.amount  Asset rule:1|18 Division: 11128746/18=618264 rewritten rule: 1|17</t>
+    <t>transfered 618264 with 220832 (tax) to income.2040.income.amount  transfer 618264 (Division: 11128746/18=618264 rewritten rule: 1|17) to income.2040.income.amount  Asset rule:1|18 Division: 11128746/18=618264 rewritten rule: 1|17</t>
   </si>
   <si>
-    <t>transfered 680090 with 149620 (tax) to income.2041.income.amount  transfer 680090 (Division: 11561530/17=680090 rewritten rule: 1|16) to income.2041.income.amount  Asset rule:1|17 Division: 11561530/17=680090 rewritten rule: 1|16</t>
+    <t>transfered 680090 with 244923 (tax) to income.2041.income.amount  transfer 680090 (Division: 11561530/17=680090 rewritten rule: 1|16) to income.2041.income.amount  Asset rule:1|17 Division: 11561530/17=680090 rewritten rule: 1|16</t>
   </si>
   <si>
-    <t>transfered 748099 with 164582 (tax) to income.2042.income.amount  transfer 748099 (Division: 11969584/16=748099 rewritten rule: 1|15) to income.2042.income.amount  Asset rule:1|16 Division: 11969584/16=748099 rewritten rule: 1|15</t>
+    <t>transfered 748099 with 276887 (tax) to income.2042.income.amount  transfer 748099 (Division: 11969584/16=748099 rewritten rule: 1|15) to income.2042.income.amount  Asset rule:1|16 Division: 11969584/16=748099 rewritten rule: 1|15</t>
   </si>
   <si>
-    <t>transfered 822909 with 181040 (tax) to income.2043.income.amount  transfer 822909 (Division: 12343634/15=822909 rewritten rule: 1|14) to income.2043.income.amount  Asset rule:1|15 Division: 12343634/15=822909 rewritten rule: 1|14</t>
+    <t>transfered 822909 with 312049 (tax) to income.2043.income.amount  transfer 822909 (Division: 12343634/15=822909 rewritten rule: 1|14) to income.2043.income.amount  Asset rule:1|15 Division: 12343634/15=822909 rewritten rule: 1|14</t>
   </si>
   <si>
-    <t>transfered 905200 with 199144 (tax) to income.2044.income.amount  transfer 905200 (Division: 12672798/14=905200 rewritten rule: 1|13) to income.2044.income.amount  Asset rule:1|14 Division: 12672798/14=905200 rewritten rule: 1|13</t>
+    <t>transfered 905200 with 350725 (tax) to income.2044.income.amount  transfer 905200 (Division: 12672798/14=905200 rewritten rule: 1|13) to income.2044.income.amount  Asset rule:1|14 Division: 12672798/14=905200 rewritten rule: 1|13</t>
   </si>
   <si>
-    <t>transfered 995720 with 219058 (tax) to income.2045.income.amount  transfer 995720 (Division: 12944358/13=995720 rewritten rule: 1|12) to income.2045.income.amount  Asset rule:1|13 Division: 12944358/13=995720 rewritten rule: 1|12</t>
+    <t>transfered 995720 with 395003 (tax) to income.2045.income.amount  transfer 995720 (Division: 12944358/13=995720 rewritten rule: 1|12) to income.2045.income.amount  Asset rule:1|13 Division: 12944358/13=995720 rewritten rule: 1|12</t>
   </si>
   <si>
-    <t>transfered 1095292 with 240964 (tax) to income.2046.income.amount  transfer 1095292 (Division: 13143502/12=1095292 rewritten rule: 1|11) to income.2046.income.amount  Asset rule:1|12 Division: 13143502/12=1095292 rewritten rule: 1|11</t>
+    <t>transfered 1095292 with 444789 (tax) to income.2046.income.amount  transfer 1095292 (Division: 13143502/12=1095292 rewritten rule: 1|11) to income.2046.income.amount  Asset rule:1|12 Division: 13143502/12=1095292 rewritten rule: 1|11</t>
   </si>
   <si>
-    <t>transfered 1204821 with 265061 (tax) to income.2047.income.amount  transfer 1204821 (Division: 13253031/11=1204821 rewritten rule: 1|10) to income.2047.income.amount  Asset rule:1|11 Division: 13253031/11=1204821 rewritten rule: 1|10</t>
+    <t>transfered 1204821 with 499555 (tax) to income.2047.income.amount  transfer 1204821 (Division: 13253031/11=1204821 rewritten rule: 1|10) to income.2047.income.amount  Asset rule:1|11 Division: 13253031/11=1204821 rewritten rule: 1|10</t>
   </si>
   <si>
-    <t>transfered 1325303 with 291567 (tax) to income.2048.income.amount  transfer 1325303 (Division: 13253031/10=1325303 rewritten rule: 1|9) to income.2048.income.amount  Asset rule:1|10 Division: 13253031/10=1325303 rewritten rule: 1|9</t>
+    <t>transfered 1325303 with 559796 (tax) to income.2048.income.amount  transfer 1325303 (Division: 13253031/10=1325303 rewritten rule: 1|9) to income.2048.income.amount  Asset rule:1|10 Division: 13253031/10=1325303 rewritten rule: 1|9</t>
   </si>
   <si>
-    <t>transfered 1457833 with 320723 (tax) to income.2049.income.amount  transfer 1457833 (Division: 13120501/9=1457833 rewritten rule: 1|8) to income.2049.income.amount  Asset rule:1|9 Division: 13120501/9=1457833 rewritten rule: 1|8</t>
+    <t>transfered 1457833 with 627139 (tax) to income.2049.income.amount  transfer 1457833 (Division: 13120501/9=1457833 rewritten rule: 1|8) to income.2049.income.amount  Asset rule:1|9 Division: 13120501/9=1457833 rewritten rule: 1|8</t>
   </si>
   <si>
-    <t>transfered 1603617 with 352796 (tax) to income.2050.income.amount  transfer 1603617 (Division: 12828935/8=1603617 rewritten rule: 1|7) to income.2050.income.amount  Asset rule:1|8 Division: 12828935/8=1603617 rewritten rule: 1|7</t>
+    <t>transfered 1603617 with 701489 (tax) to income.2050.income.amount  transfer 1603617 (Division: 12828935/8=1603617 rewritten rule: 1|7) to income.2050.income.amount  Asset rule:1|8 Division: 12828935/8=1603617 rewritten rule: 1|7</t>
   </si>
   <si>
-    <t>transfered 1763979 with 388075 (tax) to income.2051.income.amount  transfer 1763979 (Division: 12347850/7=1763979 rewritten rule: 1|6) to income.2051.income.amount  Asset rule:1|7 Division: 12347850/7=1763979 rewritten rule: 1|6</t>
+    <t>transfered 1763979 with 783273 (tax) to income.2051.income.amount  transfer 1763979 (Division: 12347850/7=1763979 rewritten rule: 1|6) to income.2051.income.amount  Asset rule:1|7 Division: 12347850/7=1763979 rewritten rule: 1|6</t>
   </si>
   <si>
-    <t>transfered 1940376 with 426883 (tax) to income.2052.income.amount  transfer 1940376 (Division: 11642258/6=1940376 rewritten rule: 1|5) to income.2052.income.amount  Asset rule:1|6 Division: 11642258/6=1940376 rewritten rule: 1|5</t>
+    <t>transfered 1940376 with 873236 (tax) to income.2052.income.amount  transfer 1940376 (Division: 11642258/6=1940376 rewritten rule: 1|5) to income.2052.income.amount  Asset rule:1|6 Division: 11642258/6=1940376 rewritten rule: 1|5</t>
   </si>
   <si>
-    <t>transfered 2134414 with 469571 (tax) to income.2053.income.amount  transfer 2134414 (Division: 10672070/5=2134414 rewritten rule: 1|4) to income.2053.income.amount  Asset rule:1|5 Division: 10672070/5=2134414 rewritten rule: 1|4</t>
+    <t>transfered 2134414 with 972195 (tax) to income.2053.income.amount  transfer 2134414 (Division: 10672070/5=2134414 rewritten rule: 1|4) to income.2053.income.amount  Asset rule:1|5 Division: 10672070/5=2134414 rewritten rule: 1|4</t>
   </si>
   <si>
-    <t>transfered 2347856 with 516528 (tax) to income.2054.income.amount  transfer 2347856 (Division: 9391422/4=2347856 rewritten rule: 1|3) to income.2054.income.amount  Asset rule:1|4 Division: 9391422/4=2347856 rewritten rule: 1|3</t>
+    <t>transfered 2347856 with 1081051 (tax) to income.2054.income.amount  transfer 2347856 (Division: 9391422/4=2347856 rewritten rule: 1|3) to income.2054.income.amount  Asset rule:1|4 Division: 9391422/4=2347856 rewritten rule: 1|3</t>
   </si>
   <si>
-    <t>transfered 2582641 with 568181 (tax) to income.2055.income.amount  transfer 2582641 (Division: 7747923/3=2582641 rewritten rule: 1|2) to income.2055.income.amount  Asset rule:1|3 Division: 7747923/3=2582641 rewritten rule: 1|2</t>
+    <t>transfered 2582641 with 1200791 (tax) to income.2055.income.amount  transfer 2582641 (Division: 7747923/3=2582641 rewritten rule: 1|2) to income.2055.income.amount  Asset rule:1|3 Division: 7747923/3=2582641 rewritten rule: 1|2</t>
   </si>
   <si>
-    <t>transfered 2840905 with 624999 (tax) to income.2056.income.amount  transfer 2840905 (Division: 5681810/2=2840905 rewritten rule: 1|1) to income.2056.income.amount  Asset rule:1|2 Division: 5681810/2=2840905 rewritten rule: 1|1</t>
+    <t>transfered 2840905 with 1332505 (tax) to income.2056.income.amount  transfer 2840905 (Division: 5681810/2=2840905 rewritten rule: 1|1) to income.2056.income.amount  Asset rule:1|2 Division: 5681810/2=2840905 rewritten rule: 1|1</t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 3124996 with 687499 (tax) to income.2057.income.amount  transfer 3124996 (Division: 3124996/1=3124996 rewritten rule: ) to income.2057.income.amount </t>
+    <t xml:space="preserve">transfered 3124996 with 1477392 (tax) to income.2057.income.amount  transfer 3124996 (Division: 3124996/1=3124996 rewritten rule: ) to income.2057.income.amount </t>
   </si>
   <si>
     <t>Income</t>
@@ -375,64 +375,64 @@
     <t>Inntekt fra investeringer, må være helt til slutt i konfigurasjonsfilen siden alle transfers til slutt havner her. Alle transfer hit er også ferdig skattet, så det skal ikke skattes i denne kategorien.</t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 510962 with 112412 (tax) from otp.2038.asset.marketAmount  transfer 510962 (Division: 10219235/20=510962 rewritten rule: 1|19) to income.2038.income.amount </t>
+    <t xml:space="preserve">transfered 510962 with 180701 (tax) from otp.2038.asset.marketAmount  transfer 510962 (Division: 10219235/20=510962 rewritten rule: 1|19) to income.2038.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 562058 with 123653 (tax) from otp.2039.asset.marketAmount  transfer 562058 (Division: 10679100/19=562058 rewritten rule: 1|18) to income.2039.income.amount </t>
+    <t xml:space="preserve">transfered 562058 with 199811 (tax) from otp.2039.asset.marketAmount  transfer 562058 (Division: 10679100/19=562058 rewritten rule: 1|18) to income.2039.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 618264 with 136018 (tax) from otp.2040.asset.marketAmount  transfer 618264 (Division: 11128746/18=618264 rewritten rule: 1|17) to income.2040.income.amount </t>
+    <t xml:space="preserve">transfered 618264 with 220832 (tax) from otp.2040.asset.marketAmount  transfer 618264 (Division: 11128746/18=618264 rewritten rule: 1|17) to income.2040.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 680090 with 149620 (tax) from otp.2041.asset.marketAmount  transfer 680090 (Division: 11561530/17=680090 rewritten rule: 1|16) to income.2041.income.amount </t>
+    <t xml:space="preserve">transfered 680090 with 244923 (tax) from otp.2041.asset.marketAmount  transfer 680090 (Division: 11561530/17=680090 rewritten rule: 1|16) to income.2041.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 748099 with 164582 (tax) from otp.2042.asset.marketAmount  transfer 748099 (Division: 11969584/16=748099 rewritten rule: 1|15) to income.2042.income.amount </t>
+    <t xml:space="preserve">transfered 748099 with 276887 (tax) from otp.2042.asset.marketAmount  transfer 748099 (Division: 11969584/16=748099 rewritten rule: 1|15) to income.2042.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 822909 with 181040 (tax) from otp.2043.asset.marketAmount  transfer 822909 (Division: 12343634/15=822909 rewritten rule: 1|14) to income.2043.income.amount </t>
+    <t xml:space="preserve">transfered 822909 with 312049 (tax) from otp.2043.asset.marketAmount  transfer 822909 (Division: 12343634/15=822909 rewritten rule: 1|14) to income.2043.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 905200 with 199144 (tax) from otp.2044.asset.marketAmount  transfer 905200 (Division: 12672798/14=905200 rewritten rule: 1|13) to income.2044.income.amount </t>
+    <t xml:space="preserve">transfered 905200 with 350725 (tax) from otp.2044.asset.marketAmount  transfer 905200 (Division: 12672798/14=905200 rewritten rule: 1|13) to income.2044.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 995720 with 219058 (tax) from otp.2045.asset.marketAmount  transfer 995720 (Division: 12944358/13=995720 rewritten rule: 1|12) to income.2045.income.amount </t>
+    <t xml:space="preserve">transfered 995720 with 395003 (tax) from otp.2045.asset.marketAmount  transfer 995720 (Division: 12944358/13=995720 rewritten rule: 1|12) to income.2045.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 1095292 with 240964 (tax) from otp.2046.asset.marketAmount  transfer 1095292 (Division: 13143502/12=1095292 rewritten rule: 1|11) to income.2046.income.amount </t>
+    <t xml:space="preserve">transfered 1095292 with 444789 (tax) from otp.2046.asset.marketAmount  transfer 1095292 (Division: 13143502/12=1095292 rewritten rule: 1|11) to income.2046.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 1204821 with 265061 (tax) from otp.2047.asset.marketAmount  transfer 1204821 (Division: 13253031/11=1204821 rewritten rule: 1|10) to income.2047.income.amount </t>
+    <t xml:space="preserve">transfered 1204821 with 499555 (tax) from otp.2047.asset.marketAmount  transfer 1204821 (Division: 13253031/11=1204821 rewritten rule: 1|10) to income.2047.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 1325303 with 291567 (tax) from otp.2048.asset.marketAmount  transfer 1325303 (Division: 13253031/10=1325303 rewritten rule: 1|9) to income.2048.income.amount </t>
+    <t xml:space="preserve">transfered 1325303 with 559796 (tax) from otp.2048.asset.marketAmount  transfer 1325303 (Division: 13253031/10=1325303 rewritten rule: 1|9) to income.2048.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 1457833 with 320723 (tax) from otp.2049.asset.marketAmount  transfer 1457833 (Division: 13120501/9=1457833 rewritten rule: 1|8) to income.2049.income.amount </t>
+    <t xml:space="preserve">transfered 1457833 with 627139 (tax) from otp.2049.asset.marketAmount  transfer 1457833 (Division: 13120501/9=1457833 rewritten rule: 1|8) to income.2049.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 1603617 with 352796 (tax) from otp.2050.asset.marketAmount  transfer 1603617 (Division: 12828935/8=1603617 rewritten rule: 1|7) to income.2050.income.amount </t>
+    <t xml:space="preserve">transfered 1603617 with 701489 (tax) from otp.2050.asset.marketAmount  transfer 1603617 (Division: 12828935/8=1603617 rewritten rule: 1|7) to income.2050.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 1763979 with 388075 (tax) from otp.2051.asset.marketAmount  transfer 1763979 (Division: 12347850/7=1763979 rewritten rule: 1|6) to income.2051.income.amount </t>
+    <t xml:space="preserve">transfered 1763979 with 783273 (tax) from otp.2051.asset.marketAmount  transfer 1763979 (Division: 12347850/7=1763979 rewritten rule: 1|6) to income.2051.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 1940376 with 426883 (tax) from otp.2052.asset.marketAmount  transfer 1940376 (Division: 11642258/6=1940376 rewritten rule: 1|5) to income.2052.income.amount </t>
+    <t xml:space="preserve">transfered 1940376 with 873236 (tax) from otp.2052.asset.marketAmount  transfer 1940376 (Division: 11642258/6=1940376 rewritten rule: 1|5) to income.2052.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 2134414 with 469571 (tax) from otp.2053.asset.marketAmount  transfer 2134414 (Division: 10672070/5=2134414 rewritten rule: 1|4) to income.2053.income.amount </t>
+    <t xml:space="preserve">transfered 2134414 with 972195 (tax) from otp.2053.asset.marketAmount  transfer 2134414 (Division: 10672070/5=2134414 rewritten rule: 1|4) to income.2053.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 2347856 with 516528 (tax) from otp.2054.asset.marketAmount  transfer 2347856 (Division: 9391422/4=2347856 rewritten rule: 1|3) to income.2054.income.amount </t>
+    <t xml:space="preserve">transfered 2347856 with 1081051 (tax) from otp.2054.asset.marketAmount  transfer 2347856 (Division: 9391422/4=2347856 rewritten rule: 1|3) to income.2054.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 2582641 with 568181 (tax) from otp.2055.asset.marketAmount  transfer 2582641 (Division: 7747923/3=2582641 rewritten rule: 1|2) to income.2055.income.amount </t>
+    <t xml:space="preserve">transfered 2582641 with 1200791 (tax) from otp.2055.asset.marketAmount  transfer 2582641 (Division: 7747923/3=2582641 rewritten rule: 1|2) to income.2055.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 2840905 with 624999 (tax) from otp.2056.asset.marketAmount  transfer 2840905 (Division: 5681810/2=2840905 rewritten rule: 1|1) to income.2056.income.amount </t>
+    <t xml:space="preserve">transfered 2840905 with 1332505 (tax) from otp.2056.asset.marketAmount  transfer 2840905 (Division: 5681810/2=2840905 rewritten rule: 1|1) to income.2056.income.amount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 3124996 with 687499 (tax) from otp.2057.asset.marketAmount  transfer 3124996 (Division: 3124996/1=3124996 rewritten rule: ) to income.2057.income.amount </t>
+    <t xml:space="preserve">transfered 3124996 with 1477392 (tax) from otp.2057.asset.marketAmount  transfer 3124996 (Division: 3124996/1=3124996 rewritten rule: ) to income.2057.income.amount </t>
   </si>
   <si>
     <t>total</t>
@@ -4162,17 +4162,17 @@
       </c>
       <c r="Z37" s="3"/>
       <c r="AA37" s="1">
-        <v>1233452.0</v>
+        <v>736181.0</v>
       </c>
       <c r="AB37" s="1">
-        <v>150900.0</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="6">
-        <v>33198.0</v>
+        <v>530469.0</v>
       </c>
       <c r="AD37" s="2"/>
       <c r="AE37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2">
@@ -4271,17 +4271,17 @@
       </c>
       <c r="Z38" s="3"/>
       <c r="AA38" s="1">
-        <v>1154267.0</v>
+        <v>841472.0</v>
       </c>
       <c r="AB38" s="1">
-        <v>1479830.0</v>
+        <v>0</v>
       </c>
       <c r="AC38" s="6">
-        <v>325563.0</v>
+        <v>638358.0</v>
       </c>
       <c r="AD38" s="2"/>
       <c r="AE38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2">
@@ -4380,17 +4380,17 @@
       </c>
       <c r="Z39" s="11"/>
       <c r="AA39" s="9">
-        <v>1343924.6</v>
+        <v>960616.6</v>
       </c>
       <c r="AB39" s="9">
-        <v>1722980.6</v>
+        <v>0</v>
       </c>
       <c r="AC39" s="9">
-        <v>379056.0</v>
+        <v>762364.0</v>
       </c>
       <c r="AD39" s="10"/>
       <c r="AE39" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF39" s="10"/>
       <c r="AG39" s="10">
@@ -4489,17 +4489,17 @@
       </c>
       <c r="Z40" s="15"/>
       <c r="AA40" s="13">
-        <v>1559969.7</v>
+        <v>1096337.7</v>
       </c>
       <c r="AB40" s="13">
-        <v>1999961.7</v>
+        <v>0</v>
       </c>
       <c r="AC40" s="13">
-        <v>439992.0</v>
+        <v>903624.0</v>
       </c>
       <c r="AD40" s="14"/>
       <c r="AE40" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF40" s="14"/>
       <c r="AG40" s="14">
@@ -4598,17 +4598,17 @@
       </c>
       <c r="Z41" s="3"/>
       <c r="AA41" s="1">
-        <v>1805786.6</v>
+        <v>1250760.6</v>
       </c>
       <c r="AB41" s="1">
-        <v>2315110.6</v>
+        <v>0</v>
       </c>
       <c r="AC41" s="6">
-        <v>509324.0</v>
+        <v>1064350.0</v>
       </c>
       <c r="AD41" s="2"/>
       <c r="AE41" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF41" s="2"/>
       <c r="AG41" s="2">
@@ -4707,17 +4707,17 @@
       </c>
       <c r="Z42" s="3"/>
       <c r="AA42" s="1">
-        <v>2085165.3</v>
+        <v>1426267.3</v>
       </c>
       <c r="AB42" s="1">
-        <v>2673289.3</v>
+        <v>0</v>
       </c>
       <c r="AC42" s="6">
-        <v>588124.0</v>
+        <v>1247022.0</v>
       </c>
       <c r="AD42" s="2"/>
       <c r="AE42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2">
@@ -4816,17 +4816,17 @@
       </c>
       <c r="Z43" s="3"/>
       <c r="AA43" s="1">
-        <v>2402361.5</v>
+        <v>1625532.5</v>
       </c>
       <c r="AB43" s="1">
-        <v>3079950.5</v>
+        <v>0</v>
       </c>
       <c r="AC43" s="6">
-        <v>677589.0</v>
+        <v>1454418.0</v>
       </c>
       <c r="AD43" s="2"/>
       <c r="AE43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF43" s="2"/>
       <c r="AG43" s="2">
@@ -4925,17 +4925,17 @@
       </c>
       <c r="Z44" s="3"/>
       <c r="AA44" s="1">
-        <v>2762146.5</v>
+        <v>1851551.5</v>
       </c>
       <c r="AB44" s="1">
-        <v>3541213.5</v>
+        <v>0</v>
       </c>
       <c r="AC44" s="6">
-        <v>779067.0</v>
+        <v>1689662.0</v>
       </c>
       <c r="AD44" s="2"/>
       <c r="AE44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF44" s="2"/>
       <c r="AG44" s="2">
@@ -5034,17 +5034,17 @@
       </c>
       <c r="Z45" s="3"/>
       <c r="AA45" s="1">
-        <v>3169864.0</v>
+        <v>2107681.0</v>
       </c>
       <c r="AB45" s="1">
-        <v>4063928.0</v>
+        <v>0</v>
       </c>
       <c r="AC45" s="6">
-        <v>894064.0</v>
+        <v>1956247.0</v>
       </c>
       <c r="AD45" s="2"/>
       <c r="AE45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF45" s="2"/>
       <c r="AG45" s="2">
@@ -5143,17 +5143,17 @@
       </c>
       <c r="Z46" s="3"/>
       <c r="AA46" s="1">
-        <v>3631504.2</v>
+        <v>2397686.2</v>
       </c>
       <c r="AB46" s="1">
-        <v>4655774.2</v>
+        <v>0</v>
       </c>
       <c r="AC46" s="6">
-        <v>1024270.0</v>
+        <v>2258088.0</v>
       </c>
       <c r="AD46" s="2"/>
       <c r="AE46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF46" s="2"/>
       <c r="AG46" s="2">
@@ -5252,17 +5252,17 @@
       </c>
       <c r="Z47" s="3"/>
       <c r="AA47" s="1">
-        <v>4153771.6</v>
+        <v>2725776.6</v>
       </c>
       <c r="AB47" s="1">
-        <v>5325348.6</v>
+        <v>0</v>
       </c>
       <c r="AC47" s="6">
-        <v>1171577.0</v>
+        <v>2599572.0</v>
       </c>
       <c r="AD47" s="2"/>
       <c r="AE47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF47" s="2"/>
       <c r="AG47" s="2">
@@ -5361,17 +5361,17 @@
       </c>
       <c r="Z48" s="3"/>
       <c r="AA48" s="1">
-        <v>4744179.7</v>
+        <v>3096674.7</v>
       </c>
       <c r="AB48" s="1">
-        <v>6082281.7</v>
+        <v>0</v>
       </c>
       <c r="AC48" s="6">
-        <v>1338102.0</v>
+        <v>2985607.0</v>
       </c>
       <c r="AD48" s="2"/>
       <c r="AE48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF48" s="2"/>
       <c r="AG48" s="2">
@@ -5470,17 +5470,17 @@
       </c>
       <c r="Z49" s="3"/>
       <c r="AA49" s="1">
-        <v>5411131.0</v>
+        <v>3515656.0</v>
       </c>
       <c r="AB49" s="1">
-        <v>6937348.0</v>
+        <v>0</v>
       </c>
       <c r="AC49" s="6">
-        <v>1526217.0</v>
+        <v>3421692.0</v>
       </c>
       <c r="AD49" s="2"/>
       <c r="AE49" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF49" s="2"/>
       <c r="AG49" s="2">
@@ -5579,17 +5579,17 @@
       </c>
       <c r="Z50" s="3"/>
       <c r="AA50" s="1">
-        <v>6164031.6</v>
+        <v>3988632.6</v>
       </c>
       <c r="AB50" s="1">
-        <v>7902604.6</v>
+        <v>0</v>
       </c>
       <c r="AC50" s="6">
-        <v>1738573.0</v>
+        <v>3913972.0</v>
       </c>
       <c r="AD50" s="2"/>
       <c r="AE50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF50" s="2"/>
       <c r="AG50" s="2">
@@ -5688,17 +5688,17 @@
       </c>
       <c r="Z51" s="3"/>
       <c r="AA51" s="1">
-        <v>7013400.7</v>
+        <v>4522210.7</v>
       </c>
       <c r="AB51" s="1">
-        <v>8991539.7</v>
+        <v>0</v>
       </c>
       <c r="AC51" s="6">
-        <v>1978139.0</v>
+        <v>4469329.0</v>
       </c>
       <c r="AD51" s="2"/>
       <c r="AE51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF51" s="2"/>
       <c r="AG51" s="2">
@@ -5797,17 +5797,17 @@
       </c>
       <c r="Z52" s="3"/>
       <c r="AA52" s="1">
-        <v>7971003.4</v>
+        <v>5123781.4</v>
       </c>
       <c r="AB52" s="1">
-        <v>10219235.4</v>
+        <v>0</v>
       </c>
       <c r="AC52" s="6">
-        <v>2248232.0</v>
+        <v>5095454.0</v>
       </c>
       <c r="AD52" s="2"/>
       <c r="AE52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF52" s="2"/>
       <c r="AG52" s="2">
@@ -5856,10 +5856,10 @@
         <v>0.1</v>
       </c>
       <c r="G53" s="16">
-        <v>1519291.0</v>
+        <v>1587580.0</v>
       </c>
       <c r="H53" s="17">
-        <v>0.43436895763126</v>
+        <v>0.45389294727359</v>
       </c>
       <c r="I53" s="16">
         <v>0</v>
@@ -5906,17 +5906,17 @@
       </c>
       <c r="Z53" s="18"/>
       <c r="AA53" s="16">
-        <v>8329698.3</v>
+        <v>5349115.3</v>
       </c>
       <c r="AB53" s="16">
-        <v>10679100.3</v>
+        <v>0</v>
       </c>
       <c r="AC53" s="16">
-        <v>2349402.0</v>
+        <v>5329985.0</v>
       </c>
       <c r="AD53" s="17"/>
       <c r="AE53" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF53" s="17"/>
       <c r="AG53" s="17">
@@ -5926,10 +5926,10 @@
         <v>1.36</v>
       </c>
       <c r="AI53" s="16">
-        <v>1579562.4</v>
+        <v>1511273.4</v>
       </c>
       <c r="AJ53" s="16">
-        <v>8348700.0</v>
+        <v>8280411.0</v>
       </c>
       <c r="AK53" s="17"/>
       <c r="AL53" s="16">
@@ -5965,10 +5965,10 @@
         <v>0.1</v>
       </c>
       <c r="G54" s="1">
-        <v>123653.0</v>
+        <v>199811.0</v>
       </c>
       <c r="H54" s="2">
-        <v>0.2200004270022</v>
+        <v>0.35549889869017</v>
       </c>
       <c r="I54" s="1">
         <v>0</v>
@@ -6015,17 +6015,17 @@
       </c>
       <c r="Z54" s="3"/>
       <c r="AA54" s="1">
-        <v>8680422.2</v>
+        <v>5569442.2</v>
       </c>
       <c r="AB54" s="1">
-        <v>11128746.2</v>
+        <v>0</v>
       </c>
       <c r="AC54" s="6">
-        <v>2448324.0</v>
+        <v>5559304.0</v>
       </c>
       <c r="AD54" s="2"/>
       <c r="AE54" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF54" s="2"/>
       <c r="AG54" s="2">
@@ -6035,10 +6035,10 @@
         <v>0.33</v>
       </c>
       <c r="AI54" s="7">
-        <v>-323.60000000009</v>
+        <v>-76481.6</v>
       </c>
       <c r="AJ54" s="1">
-        <v>8348376.4</v>
+        <v>8203929.4</v>
       </c>
       <c r="AK54" s="2"/>
       <c r="AL54" s="1">
@@ -6074,10 +6074,10 @@
         <v>0.1</v>
       </c>
       <c r="G55" s="1">
-        <v>136018.0</v>
+        <v>220832.0</v>
       </c>
       <c r="H55" s="2">
-        <v>0.21999987060544</v>
+        <v>0.35718075126483</v>
       </c>
       <c r="I55" s="1">
         <v>0</v>
@@ -6124,17 +6124,17 @@
       </c>
       <c r="Z55" s="3"/>
       <c r="AA55" s="1">
-        <v>9017993.2</v>
+        <v>5781506.2</v>
       </c>
       <c r="AB55" s="1">
-        <v>11561530.2</v>
+        <v>0</v>
       </c>
       <c r="AC55" s="6">
-        <v>2543537.0</v>
+        <v>5780024.0</v>
       </c>
       <c r="AD55" s="2"/>
       <c r="AE55" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF55" s="2"/>
       <c r="AG55" s="2">
@@ -6144,10 +6144,10 @@
         <v>0.68</v>
       </c>
       <c r="AI55" s="7">
-        <v>-355.70000000019</v>
+        <v>-85169.7</v>
       </c>
       <c r="AJ55" s="1">
-        <v>8348020.7</v>
+        <v>8118759.7</v>
       </c>
       <c r="AK55" s="2"/>
       <c r="AL55" s="1">
@@ -6183,10 +6183,10 @@
         <v>0.1</v>
       </c>
       <c r="G56" s="1">
-        <v>149620.0</v>
+        <v>244923.0</v>
       </c>
       <c r="H56" s="2">
-        <v>0.22000029407872</v>
+        <v>0.36013321766237</v>
       </c>
       <c r="I56" s="1">
         <v>0</v>
@@ -6233,17 +6233,17 @@
       </c>
       <c r="Z56" s="3"/>
       <c r="AA56" s="1">
-        <v>9336276.0</v>
+        <v>5981452.0</v>
       </c>
       <c r="AB56" s="1">
-        <v>11969584.0</v>
+        <v>0</v>
       </c>
       <c r="AC56" s="6">
-        <v>2633308.0</v>
+        <v>5988132.0</v>
       </c>
       <c r="AD56" s="2"/>
       <c r="AE56" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF56" s="2"/>
       <c r="AG56" s="2">
@@ -6253,10 +6253,10 @@
         <v>17.94</v>
       </c>
       <c r="AI56" s="7">
-        <v>-392.60000000009</v>
+        <v>-95695.6</v>
       </c>
       <c r="AJ56" s="1">
-        <v>8347628.1</v>
+        <v>8023064.1</v>
       </c>
       <c r="AK56" s="2"/>
       <c r="AL56" s="1">
@@ -6292,10 +6292,10 @@
         <v>0.1</v>
       </c>
       <c r="G57" s="16">
-        <v>164582.0</v>
+        <v>276887.0</v>
       </c>
       <c r="H57" s="17">
-        <v>0.22000029407872</v>
+        <v>0.37012079951985</v>
       </c>
       <c r="I57" s="16">
         <v>0</v>
@@ -6342,26 +6342,26 @@
       </c>
       <c r="Z57" s="18"/>
       <c r="AA57" s="16">
-        <v>9628034.5</v>
+        <v>6164737.5</v>
       </c>
       <c r="AB57" s="16">
-        <v>12343633.5</v>
+        <v>0</v>
       </c>
       <c r="AC57" s="16">
-        <v>2715599.0</v>
+        <v>6178896.0</v>
       </c>
       <c r="AD57" s="17"/>
       <c r="AE57" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF57" s="17"/>
       <c r="AG57" s="17"/>
       <c r="AH57" s="17"/>
       <c r="AI57" s="16">
-        <v>-432.30000000005</v>
+        <v>-112737.3</v>
       </c>
       <c r="AJ57" s="16">
-        <v>8347195.8</v>
+        <v>7910326.8</v>
       </c>
       <c r="AK57" s="17"/>
       <c r="AL57" s="16">
@@ -6397,10 +6397,10 @@
         <v>0.09</v>
       </c>
       <c r="G58" s="1">
-        <v>181040.0</v>
+        <v>312049.0</v>
       </c>
       <c r="H58" s="2">
-        <v>0.22000002430402</v>
+        <v>0.37920231763172</v>
       </c>
       <c r="I58" s="1">
         <v>0</v>
@@ -6447,26 +6447,26 @@
       </c>
       <c r="Z58" s="3"/>
       <c r="AA58" s="1">
-        <v>9884782.5</v>
+        <v>6326027.5</v>
       </c>
       <c r="AB58" s="1">
-        <v>12672797.5</v>
+        <v>0</v>
       </c>
       <c r="AC58" s="6">
-        <v>2788015.0</v>
+        <v>6346770.0</v>
       </c>
       <c r="AD58" s="2"/>
       <c r="AE58" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF58" s="2"/>
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="7">
-        <v>-474.80000000005</v>
+        <v>-131483.8</v>
       </c>
       <c r="AJ58" s="1">
-        <v>8346721.0</v>
+        <v>7778843.0</v>
       </c>
       <c r="AK58" s="2"/>
       <c r="AL58" s="1">
@@ -6502,10 +6502,10 @@
         <v>0.1</v>
       </c>
       <c r="G59" s="1">
-        <v>199144.0</v>
+        <v>350725.0</v>
       </c>
       <c r="H59" s="2">
-        <v>0.22</v>
+        <v>0.38745581087053</v>
       </c>
       <c r="I59" s="1">
         <v>0</v>
@@ -6552,26 +6552,26 @@
       </c>
       <c r="Z59" s="3"/>
       <c r="AA59" s="1">
-        <v>10096598.8</v>
+        <v>6459090.8</v>
       </c>
       <c r="AB59" s="1">
-        <v>12944357.8</v>
+        <v>0</v>
       </c>
       <c r="AC59" s="6">
-        <v>2847759.0</v>
+        <v>6485267.0</v>
       </c>
       <c r="AD59" s="2"/>
       <c r="AE59" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF59" s="2"/>
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
       <c r="AI59" s="7">
-        <v>-522.30000000005</v>
+        <v>-152103.3</v>
       </c>
       <c r="AJ59" s="1">
-        <v>8346198.7</v>
+        <v>7626739.7</v>
       </c>
       <c r="AK59" s="2"/>
       <c r="AL59" s="1">
@@ -6607,10 +6607,10 @@
         <v>0.09</v>
       </c>
       <c r="G60" s="1">
-        <v>219058.0</v>
+        <v>395003.0</v>
       </c>
       <c r="H60" s="2">
-        <v>0.21999959828064</v>
+        <v>0.3967008797654</v>
       </c>
       <c r="I60" s="1">
         <v>0</v>
@@ -6657,26 +6657,26 @@
       </c>
       <c r="Z60" s="3"/>
       <c r="AA60" s="1">
-        <v>10251931.8</v>
+        <v>6556672.8</v>
       </c>
       <c r="AB60" s="1">
-        <v>13143501.8</v>
+        <v>0</v>
       </c>
       <c r="AC60" s="6">
-        <v>2891570.0</v>
+        <v>6586829.0</v>
       </c>
       <c r="AD60" s="2"/>
       <c r="AE60" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF60" s="2"/>
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="7">
-        <v>-573.80000000005</v>
+        <v>-176518.8</v>
       </c>
       <c r="AJ60" s="1">
-        <v>8345624.9</v>
+        <v>7450220.9</v>
       </c>
       <c r="AK60" s="2"/>
       <c r="AL60" s="1">
@@ -6712,10 +6712,10 @@
         <v>0.1</v>
       </c>
       <c r="G61" s="1">
-        <v>240964.0</v>
+        <v>444789.0</v>
       </c>
       <c r="H61" s="2">
-        <v>0.21999978088035</v>
+        <v>0.40609170887763</v>
       </c>
       <c r="I61" s="1">
         <v>0</v>
@@ -6762,26 +6762,26 @@
       </c>
       <c r="Z61" s="3"/>
       <c r="AA61" s="1">
-        <v>10337364.0</v>
+        <v>6610341.0</v>
       </c>
       <c r="AB61" s="1">
-        <v>13253031.0</v>
+        <v>0</v>
       </c>
       <c r="AC61" s="6">
-        <v>2915667.0</v>
+        <v>6642690.0</v>
       </c>
       <c r="AD61" s="2"/>
       <c r="AE61" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF61" s="2"/>
       <c r="AG61" s="2"/>
       <c r="AH61" s="2"/>
       <c r="AI61" s="7">
-        <v>-631.60000000009</v>
+        <v>-204456.6</v>
       </c>
       <c r="AJ61" s="1">
-        <v>8344993.3</v>
+        <v>7245764.3</v>
       </c>
       <c r="AK61" s="2"/>
       <c r="AL61" s="1">
@@ -6817,10 +6817,10 @@
         <v>0.1</v>
       </c>
       <c r="G62" s="1">
-        <v>265061.0</v>
+        <v>499555.0</v>
       </c>
       <c r="H62" s="2">
-        <v>0.22000031539955</v>
+        <v>0.41463005707902</v>
       </c>
       <c r="I62" s="1">
         <v>0</v>
@@ -6865,26 +6865,26 @@
       </c>
       <c r="Z62" s="3"/>
       <c r="AA62" s="1">
-        <v>10337364.0</v>
+        <v>6610341.0</v>
       </c>
       <c r="AB62" s="1">
-        <v>13253031.0</v>
+        <v>0</v>
       </c>
       <c r="AC62" s="6">
-        <v>2915667.0</v>
+        <v>6642690.0</v>
       </c>
       <c r="AD62" s="2"/>
       <c r="AE62" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF62" s="2"/>
       <c r="AG62" s="2"/>
       <c r="AH62" s="2"/>
       <c r="AI62" s="7">
-        <v>-696.20000000019</v>
+        <v>-235190.2</v>
       </c>
       <c r="AJ62" s="1">
-        <v>8344297.1</v>
+        <v>7010574.1</v>
       </c>
       <c r="AK62" s="2"/>
       <c r="AL62" s="1">
@@ -6920,10 +6920,10 @@
         <v>0.09</v>
       </c>
       <c r="G63" s="1">
-        <v>291567.0</v>
+        <v>559796.0</v>
       </c>
       <c r="H63" s="2">
-        <v>0.22000025654511</v>
+        <v>0.42239095512498</v>
       </c>
       <c r="I63" s="1">
         <v>0</v>
@@ -6970,26 +6970,26 @@
       </c>
       <c r="Z63" s="3"/>
       <c r="AA63" s="1">
-        <v>10233990.8</v>
+        <v>6545401.8</v>
       </c>
       <c r="AB63" s="1">
-        <v>13120500.8</v>
+        <v>0</v>
       </c>
       <c r="AC63" s="6">
-        <v>2886510.0</v>
+        <v>6575099.0</v>
       </c>
       <c r="AD63" s="2"/>
       <c r="AE63" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF63" s="2"/>
       <c r="AG63" s="2"/>
       <c r="AH63" s="2"/>
       <c r="AI63" s="7">
-        <v>-765.70000000019</v>
+        <v>-268994.7</v>
       </c>
       <c r="AJ63" s="1">
-        <v>8343531.4</v>
+        <v>6741579.4</v>
       </c>
       <c r="AK63" s="2"/>
       <c r="AL63" s="1">
@@ -7025,10 +7025,10 @@
         <v>0.1</v>
       </c>
       <c r="G64" s="1">
-        <v>320723.0</v>
+        <v>627139.0</v>
       </c>
       <c r="H64" s="2">
-        <v>0.2199998216531</v>
+        <v>0.43018576201801</v>
       </c>
       <c r="I64" s="1">
         <v>0</v>
@@ -7075,26 +7075,26 @@
       </c>
       <c r="Z64" s="3"/>
       <c r="AA64" s="1">
-        <v>10006568.8</v>
+        <v>6402535.8</v>
       </c>
       <c r="AB64" s="1">
-        <v>12828934.8</v>
+        <v>0</v>
       </c>
       <c r="AC64" s="6">
-        <v>2822366.0</v>
+        <v>6426399.0</v>
       </c>
       <c r="AD64" s="2"/>
       <c r="AE64" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF64" s="2"/>
       <c r="AG64" s="2"/>
       <c r="AH64" s="2"/>
       <c r="AI64" s="7">
-        <v>-842.5</v>
+        <v>-307258.5</v>
       </c>
       <c r="AJ64" s="1">
-        <v>8342688.9</v>
+        <v>6434320.9</v>
       </c>
       <c r="AK64" s="2"/>
       <c r="AL64" s="1">
@@ -7130,10 +7130,10 @@
         <v>0.1</v>
       </c>
       <c r="G65" s="1">
-        <v>352796.0</v>
+        <v>701489.0</v>
       </c>
       <c r="H65" s="2">
-        <v>0.22000016213348</v>
+        <v>0.4374417332817</v>
       </c>
       <c r="I65" s="1">
         <v>0</v>
@@ -7180,26 +7180,26 @@
       </c>
       <c r="Z65" s="3"/>
       <c r="AA65" s="1">
-        <v>9631322.8</v>
+        <v>6166802.8</v>
       </c>
       <c r="AB65" s="1">
-        <v>12347849.8</v>
+        <v>0</v>
       </c>
       <c r="AC65" s="6">
-        <v>2716527.0</v>
+        <v>6181047.0</v>
       </c>
       <c r="AD65" s="2"/>
       <c r="AE65" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF65" s="2"/>
       <c r="AG65" s="2"/>
       <c r="AH65" s="2"/>
       <c r="AI65" s="7">
-        <v>-926.60000000009</v>
+        <v>-349619.6</v>
       </c>
       <c r="AJ65" s="1">
-        <v>8341762.3</v>
+        <v>6084701.3</v>
       </c>
       <c r="AK65" s="2"/>
       <c r="AL65" s="1">
@@ -7235,10 +7235,10 @@
         <v>0.1</v>
       </c>
       <c r="G66" s="1">
-        <v>388075.0</v>
+        <v>783273.0</v>
       </c>
       <c r="H66" s="2">
-        <v>0.21999978457793</v>
+        <v>0.44403759908706</v>
       </c>
       <c r="I66" s="1">
         <v>0</v>
@@ -7285,26 +7285,26 @@
       </c>
       <c r="Z66" s="3"/>
       <c r="AA66" s="1">
-        <v>9080961.1</v>
+        <v>5821063.1</v>
       </c>
       <c r="AB66" s="1">
-        <v>11642258.1</v>
+        <v>0</v>
       </c>
       <c r="AC66" s="6">
-        <v>2561297.0</v>
+        <v>5821195.0</v>
       </c>
       <c r="AD66" s="2"/>
       <c r="AE66" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF66" s="2"/>
       <c r="AG66" s="2"/>
       <c r="AH66" s="2"/>
       <c r="AI66" s="7">
-        <v>-1018.5000000005</v>
+        <v>-396216.5</v>
       </c>
       <c r="AJ66" s="1">
-        <v>8340743.8</v>
+        <v>5688484.8</v>
       </c>
       <c r="AK66" s="2"/>
       <c r="AL66" s="1">
@@ -7340,10 +7340,10 @@
         <v>0.1</v>
       </c>
       <c r="G67" s="1">
-        <v>426883.0</v>
+        <v>873236.0</v>
       </c>
       <c r="H67" s="2">
-        <v>0.22000014430193</v>
+        <v>0.45003442631737</v>
       </c>
       <c r="I67" s="1">
         <v>0</v>
@@ -7390,26 +7390,26 @@
       </c>
       <c r="Z67" s="3"/>
       <c r="AA67" s="1">
-        <v>8324215.2</v>
+        <v>5345671.2</v>
       </c>
       <c r="AB67" s="1">
-        <v>10672070.2</v>
+        <v>0</v>
       </c>
       <c r="AC67" s="6">
-        <v>2347855.0</v>
+        <v>5326399.0</v>
       </c>
       <c r="AD67" s="2"/>
       <c r="AE67" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF67" s="2"/>
       <c r="AG67" s="2"/>
       <c r="AH67" s="2"/>
       <c r="AI67" s="7">
-        <v>-1123.2000000002</v>
+        <v>-447476.2</v>
       </c>
       <c r="AJ67" s="1">
-        <v>8339620.6</v>
+        <v>5241008.6</v>
       </c>
       <c r="AK67" s="2"/>
       <c r="AL67" s="1">
@@ -7445,10 +7445,10 @@
         <v>0.09</v>
       </c>
       <c r="G68" s="1">
-        <v>469571.0</v>
+        <v>972195.0</v>
       </c>
       <c r="H68" s="2">
-        <v>0.21999996251899</v>
+        <v>0.45548567428812</v>
       </c>
       <c r="I68" s="1">
         <v>0</v>
@@ -7495,26 +7495,26 @@
       </c>
       <c r="Z68" s="3"/>
       <c r="AA68" s="1">
-        <v>7325308.6</v>
+        <v>4718152.6</v>
       </c>
       <c r="AB68" s="1">
-        <v>9391421.6</v>
+        <v>0</v>
       </c>
       <c r="AC68" s="6">
-        <v>2066113.0</v>
+        <v>4673269.0</v>
       </c>
       <c r="AD68" s="2"/>
       <c r="AE68" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF68" s="2"/>
       <c r="AG68" s="2"/>
       <c r="AH68" s="2"/>
       <c r="AI68" s="7">
-        <v>-1234.2000000002</v>
+        <v>-503858.2</v>
       </c>
       <c r="AJ68" s="1">
-        <v>8338386.4</v>
+        <v>4737150.4</v>
       </c>
       <c r="AK68" s="2"/>
       <c r="AL68" s="1">
@@ -7550,10 +7550,10 @@
         <v>0.09</v>
       </c>
       <c r="G69" s="1">
-        <v>516528.0</v>
+        <v>1081051.0</v>
       </c>
       <c r="H69" s="2">
-        <v>0.21999986370544</v>
+        <v>0.46044178177878</v>
       </c>
       <c r="I69" s="1">
         <v>0</v>
@@ -7600,26 +7600,26 @@
       </c>
       <c r="Z69" s="3"/>
       <c r="AA69" s="1">
-        <v>6043379.6</v>
+        <v>3912838.6</v>
       </c>
       <c r="AB69" s="1">
-        <v>7747922.6</v>
+        <v>0</v>
       </c>
       <c r="AC69" s="6">
-        <v>1704543.0</v>
+        <v>3835084.0</v>
       </c>
       <c r="AD69" s="2"/>
       <c r="AE69" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF69" s="2"/>
       <c r="AG69" s="2"/>
       <c r="AH69" s="2"/>
       <c r="AI69" s="7">
-        <v>-1356.1000000006</v>
+        <v>-565879.1</v>
       </c>
       <c r="AJ69" s="1">
-        <v>8337030.3</v>
+        <v>4171271.3</v>
       </c>
       <c r="AK69" s="2"/>
       <c r="AL69" s="1">
@@ -7655,10 +7655,10 @@
         <v>0.09</v>
       </c>
       <c r="G70" s="1">
-        <v>568181.0</v>
+        <v>1200791.0</v>
       </c>
       <c r="H70" s="2">
-        <v>0.21999999225599</v>
+        <v>0.46494692835744</v>
       </c>
       <c r="I70" s="1">
         <v>0</v>
@@ -7705,26 +7705,26 @@
       </c>
       <c r="Z70" s="3"/>
       <c r="AA70" s="1">
-        <v>4431812.2</v>
+        <v>2900443.2</v>
       </c>
       <c r="AB70" s="1">
-        <v>5681810.2</v>
+        <v>0</v>
       </c>
       <c r="AC70" s="6">
-        <v>1249998.0</v>
+        <v>2781367.0</v>
       </c>
       <c r="AD70" s="2"/>
       <c r="AE70" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF70" s="2"/>
       <c r="AG70" s="2"/>
       <c r="AH70" s="2"/>
       <c r="AI70" s="7">
-        <v>-1493.0</v>
+        <v>-634103.0</v>
       </c>
       <c r="AJ70" s="1">
-        <v>8335537.3</v>
+        <v>3537168.3</v>
       </c>
       <c r="AK70" s="2"/>
       <c r="AL70" s="1">
@@ -7760,10 +7760,10 @@
         <v>0.1</v>
       </c>
       <c r="G71" s="1">
-        <v>624999.0</v>
+        <v>1332505.0</v>
       </c>
       <c r="H71" s="2">
-        <v>0.21999996479995</v>
+        <v>0.46904243542111</v>
       </c>
       <c r="I71" s="1">
         <v>0</v>
@@ -7810,26 +7810,26 @@
       </c>
       <c r="Z71" s="3"/>
       <c r="AA71" s="1">
-        <v>2437496.5</v>
+        <v>1647604.5</v>
       </c>
       <c r="AB71" s="1">
-        <v>3124995.5</v>
+        <v>0</v>
       </c>
       <c r="AC71" s="6">
-        <v>687499.0</v>
+        <v>1477391.0</v>
       </c>
       <c r="AD71" s="2"/>
       <c r="AE71" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF71" s="2"/>
       <c r="AG71" s="2"/>
       <c r="AH71" s="2"/>
       <c r="AI71" s="7">
-        <v>-1642.4000000004</v>
+        <v>-709148.4</v>
       </c>
       <c r="AJ71" s="1">
-        <v>8333894.9</v>
+        <v>2828019.9</v>
       </c>
       <c r="AK71" s="2"/>
       <c r="AL71" s="1">
@@ -7865,10 +7865,10 @@
         <v>0.09</v>
       </c>
       <c r="G72" s="6">
-        <v>687499.0</v>
+        <v>1477392.0</v>
       </c>
       <c r="H72" s="20">
-        <v>0.21999996159995</v>
+        <v>0.47276604514054</v>
       </c>
       <c r="I72" s="6">
         <v>0</v>
@@ -7929,10 +7929,10 @@
       <c r="AG72" s="20"/>
       <c r="AH72" s="20"/>
       <c r="AI72" s="6">
-        <v>-1805.3000000007</v>
+        <v>-791698.3</v>
       </c>
       <c r="AJ72" s="6">
-        <v>8332089.6</v>
+        <v>2036321.6</v>
       </c>
       <c r="AK72" s="20"/>
       <c r="AL72" s="6">
@@ -11639,17 +11639,17 @@
       </c>
       <c r="Z37" s="3"/>
       <c r="AA37" s="1">
-        <v>1233452.0</v>
+        <v>736181.0</v>
       </c>
       <c r="AB37" s="1">
-        <v>150900.0</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="6">
-        <v>33198.0</v>
+        <v>530469.0</v>
       </c>
       <c r="AD37" s="2"/>
       <c r="AE37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2">
@@ -11748,17 +11748,17 @@
       </c>
       <c r="Z38" s="3"/>
       <c r="AA38" s="1">
-        <v>1154267.0</v>
+        <v>841472.0</v>
       </c>
       <c r="AB38" s="1">
-        <v>1479830.0</v>
+        <v>0</v>
       </c>
       <c r="AC38" s="6">
-        <v>325563.0</v>
+        <v>638358.0</v>
       </c>
       <c r="AD38" s="2"/>
       <c r="AE38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2">
@@ -11857,17 +11857,17 @@
       </c>
       <c r="Z39" s="11"/>
       <c r="AA39" s="9">
-        <v>1343924.6</v>
+        <v>960616.6</v>
       </c>
       <c r="AB39" s="9">
-        <v>1722980.6</v>
+        <v>0</v>
       </c>
       <c r="AC39" s="9">
-        <v>379056.0</v>
+        <v>762364.0</v>
       </c>
       <c r="AD39" s="10"/>
       <c r="AE39" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF39" s="10"/>
       <c r="AG39" s="10">
@@ -11966,17 +11966,17 @@
       </c>
       <c r="Z40" s="15"/>
       <c r="AA40" s="13">
-        <v>1559969.7</v>
+        <v>1096337.7</v>
       </c>
       <c r="AB40" s="13">
-        <v>1999961.7</v>
+        <v>0</v>
       </c>
       <c r="AC40" s="13">
-        <v>439992.0</v>
+        <v>903624.0</v>
       </c>
       <c r="AD40" s="14"/>
       <c r="AE40" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF40" s="14"/>
       <c r="AG40" s="14">
@@ -12075,17 +12075,17 @@
       </c>
       <c r="Z41" s="3"/>
       <c r="AA41" s="1">
-        <v>1805786.6</v>
+        <v>1250760.6</v>
       </c>
       <c r="AB41" s="1">
-        <v>2315110.6</v>
+        <v>0</v>
       </c>
       <c r="AC41" s="6">
-        <v>509324.0</v>
+        <v>1064350.0</v>
       </c>
       <c r="AD41" s="2"/>
       <c r="AE41" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF41" s="2"/>
       <c r="AG41" s="2">
@@ -12184,17 +12184,17 @@
       </c>
       <c r="Z42" s="3"/>
       <c r="AA42" s="1">
-        <v>2085165.3</v>
+        <v>1426267.3</v>
       </c>
       <c r="AB42" s="1">
-        <v>2673289.3</v>
+        <v>0</v>
       </c>
       <c r="AC42" s="6">
-        <v>588124.0</v>
+        <v>1247022.0</v>
       </c>
       <c r="AD42" s="2"/>
       <c r="AE42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2">
@@ -12293,17 +12293,17 @@
       </c>
       <c r="Z43" s="3"/>
       <c r="AA43" s="1">
-        <v>2402361.5</v>
+        <v>1625532.5</v>
       </c>
       <c r="AB43" s="1">
-        <v>3079950.5</v>
+        <v>0</v>
       </c>
       <c r="AC43" s="6">
-        <v>677589.0</v>
+        <v>1454418.0</v>
       </c>
       <c r="AD43" s="2"/>
       <c r="AE43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF43" s="2"/>
       <c r="AG43" s="2">
@@ -12402,17 +12402,17 @@
       </c>
       <c r="Z44" s="3"/>
       <c r="AA44" s="1">
-        <v>2762146.5</v>
+        <v>1851551.5</v>
       </c>
       <c r="AB44" s="1">
-        <v>3541213.5</v>
+        <v>0</v>
       </c>
       <c r="AC44" s="6">
-        <v>779067.0</v>
+        <v>1689662.0</v>
       </c>
       <c r="AD44" s="2"/>
       <c r="AE44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF44" s="2"/>
       <c r="AG44" s="2">
@@ -12511,17 +12511,17 @@
       </c>
       <c r="Z45" s="3"/>
       <c r="AA45" s="1">
-        <v>3169864.0</v>
+        <v>2107681.0</v>
       </c>
       <c r="AB45" s="1">
-        <v>4063928.0</v>
+        <v>0</v>
       </c>
       <c r="AC45" s="6">
-        <v>894064.0</v>
+        <v>1956247.0</v>
       </c>
       <c r="AD45" s="2"/>
       <c r="AE45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF45" s="2"/>
       <c r="AG45" s="2">
@@ -12620,17 +12620,17 @@
       </c>
       <c r="Z46" s="3"/>
       <c r="AA46" s="1">
-        <v>3631504.2</v>
+        <v>2397686.2</v>
       </c>
       <c r="AB46" s="1">
-        <v>4655774.2</v>
+        <v>0</v>
       </c>
       <c r="AC46" s="6">
-        <v>1024270.0</v>
+        <v>2258088.0</v>
       </c>
       <c r="AD46" s="2"/>
       <c r="AE46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF46" s="2"/>
       <c r="AG46" s="2">
@@ -12729,17 +12729,17 @@
       </c>
       <c r="Z47" s="3"/>
       <c r="AA47" s="1">
-        <v>4153771.6</v>
+        <v>2725776.6</v>
       </c>
       <c r="AB47" s="1">
-        <v>5325348.6</v>
+        <v>0</v>
       </c>
       <c r="AC47" s="6">
-        <v>1171577.0</v>
+        <v>2599572.0</v>
       </c>
       <c r="AD47" s="2"/>
       <c r="AE47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF47" s="2"/>
       <c r="AG47" s="2">
@@ -12838,17 +12838,17 @@
       </c>
       <c r="Z48" s="3"/>
       <c r="AA48" s="1">
-        <v>4744179.7</v>
+        <v>3096674.7</v>
       </c>
       <c r="AB48" s="1">
-        <v>6082281.7</v>
+        <v>0</v>
       </c>
       <c r="AC48" s="6">
-        <v>1338102.0</v>
+        <v>2985607.0</v>
       </c>
       <c r="AD48" s="2"/>
       <c r="AE48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF48" s="2"/>
       <c r="AG48" s="2">
@@ -12947,17 +12947,17 @@
       </c>
       <c r="Z49" s="3"/>
       <c r="AA49" s="1">
-        <v>5411131.0</v>
+        <v>3515656.0</v>
       </c>
       <c r="AB49" s="1">
-        <v>6937348.0</v>
+        <v>0</v>
       </c>
       <c r="AC49" s="6">
-        <v>1526217.0</v>
+        <v>3421692.0</v>
       </c>
       <c r="AD49" s="2"/>
       <c r="AE49" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF49" s="2"/>
       <c r="AG49" s="2">
@@ -13056,17 +13056,17 @@
       </c>
       <c r="Z50" s="3"/>
       <c r="AA50" s="1">
-        <v>6164031.6</v>
+        <v>3988632.6</v>
       </c>
       <c r="AB50" s="1">
-        <v>7902604.6</v>
+        <v>0</v>
       </c>
       <c r="AC50" s="6">
-        <v>1738573.0</v>
+        <v>3913972.0</v>
       </c>
       <c r="AD50" s="2"/>
       <c r="AE50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF50" s="2"/>
       <c r="AG50" s="2">
@@ -13165,17 +13165,17 @@
       </c>
       <c r="Z51" s="3"/>
       <c r="AA51" s="1">
-        <v>7013400.7</v>
+        <v>4522210.7</v>
       </c>
       <c r="AB51" s="1">
-        <v>8991539.7</v>
+        <v>0</v>
       </c>
       <c r="AC51" s="6">
-        <v>1978139.0</v>
+        <v>4469329.0</v>
       </c>
       <c r="AD51" s="2"/>
       <c r="AE51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF51" s="2"/>
       <c r="AG51" s="2">
@@ -13274,17 +13274,17 @@
       </c>
       <c r="Z52" s="3"/>
       <c r="AA52" s="1">
-        <v>7971003.4</v>
+        <v>5123781.4</v>
       </c>
       <c r="AB52" s="1">
-        <v>10219235.4</v>
+        <v>0</v>
       </c>
       <c r="AC52" s="6">
-        <v>2248232.0</v>
+        <v>5095454.0</v>
       </c>
       <c r="AD52" s="2"/>
       <c r="AE52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF52" s="2"/>
       <c r="AG52" s="2">
@@ -13333,10 +13333,10 @@
         <v>0.1</v>
       </c>
       <c r="G53" s="16">
-        <v>1519291.0</v>
+        <v>1587580.0</v>
       </c>
       <c r="H53" s="17">
-        <v>0.43436895763126</v>
+        <v>0.45389294727359</v>
       </c>
       <c r="I53" s="16">
         <v>0</v>
@@ -13383,17 +13383,17 @@
       </c>
       <c r="Z53" s="18"/>
       <c r="AA53" s="16">
-        <v>8329698.3</v>
+        <v>5349115.3</v>
       </c>
       <c r="AB53" s="16">
-        <v>10679100.3</v>
+        <v>0</v>
       </c>
       <c r="AC53" s="16">
-        <v>2349402.0</v>
+        <v>5329985.0</v>
       </c>
       <c r="AD53" s="17"/>
       <c r="AE53" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF53" s="17"/>
       <c r="AG53" s="17">
@@ -13403,10 +13403,10 @@
         <v>1.36</v>
       </c>
       <c r="AI53" s="16">
-        <v>1579562.4</v>
+        <v>1511273.4</v>
       </c>
       <c r="AJ53" s="16">
-        <v>8348700.0</v>
+        <v>8280411.0</v>
       </c>
       <c r="AK53" s="17"/>
       <c r="AL53" s="16">
@@ -13442,10 +13442,10 @@
         <v>0.1</v>
       </c>
       <c r="G54" s="1">
-        <v>123653.0</v>
+        <v>199811.0</v>
       </c>
       <c r="H54" s="2">
-        <v>0.2200004270022</v>
+        <v>0.35549889869017</v>
       </c>
       <c r="I54" s="1">
         <v>0</v>
@@ -13492,17 +13492,17 @@
       </c>
       <c r="Z54" s="3"/>
       <c r="AA54" s="1">
-        <v>8680422.2</v>
+        <v>5569442.2</v>
       </c>
       <c r="AB54" s="1">
-        <v>11128746.2</v>
+        <v>0</v>
       </c>
       <c r="AC54" s="6">
-        <v>2448324.0</v>
+        <v>5559304.0</v>
       </c>
       <c r="AD54" s="2"/>
       <c r="AE54" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF54" s="2"/>
       <c r="AG54" s="2">
@@ -13512,10 +13512,10 @@
         <v>0.33</v>
       </c>
       <c r="AI54" s="7">
-        <v>-323.60000000009</v>
+        <v>-76481.6</v>
       </c>
       <c r="AJ54" s="1">
-        <v>8348376.4</v>
+        <v>8203929.4</v>
       </c>
       <c r="AK54" s="2"/>
       <c r="AL54" s="1">
@@ -13551,10 +13551,10 @@
         <v>0.1</v>
       </c>
       <c r="G55" s="1">
-        <v>136018.0</v>
+        <v>220832.0</v>
       </c>
       <c r="H55" s="2">
-        <v>0.21999987060544</v>
+        <v>0.35718075126483</v>
       </c>
       <c r="I55" s="1">
         <v>0</v>
@@ -13601,17 +13601,17 @@
       </c>
       <c r="Z55" s="3"/>
       <c r="AA55" s="1">
-        <v>9017993.2</v>
+        <v>5781506.2</v>
       </c>
       <c r="AB55" s="1">
-        <v>11561530.2</v>
+        <v>0</v>
       </c>
       <c r="AC55" s="6">
-        <v>2543537.0</v>
+        <v>5780024.0</v>
       </c>
       <c r="AD55" s="2"/>
       <c r="AE55" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF55" s="2"/>
       <c r="AG55" s="2">
@@ -13621,10 +13621,10 @@
         <v>0.68</v>
       </c>
       <c r="AI55" s="7">
-        <v>-355.70000000019</v>
+        <v>-85169.7</v>
       </c>
       <c r="AJ55" s="1">
-        <v>8348020.7</v>
+        <v>8118759.7</v>
       </c>
       <c r="AK55" s="2"/>
       <c r="AL55" s="1">
@@ -13660,10 +13660,10 @@
         <v>0.1</v>
       </c>
       <c r="G56" s="1">
-        <v>149620.0</v>
+        <v>244923.0</v>
       </c>
       <c r="H56" s="2">
-        <v>0.22000029407872</v>
+        <v>0.36013321766237</v>
       </c>
       <c r="I56" s="1">
         <v>0</v>
@@ -13710,17 +13710,17 @@
       </c>
       <c r="Z56" s="3"/>
       <c r="AA56" s="1">
-        <v>9336276.0</v>
+        <v>5981452.0</v>
       </c>
       <c r="AB56" s="1">
-        <v>11969584.0</v>
+        <v>0</v>
       </c>
       <c r="AC56" s="6">
-        <v>2633308.0</v>
+        <v>5988132.0</v>
       </c>
       <c r="AD56" s="2"/>
       <c r="AE56" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF56" s="2"/>
       <c r="AG56" s="2">
@@ -13730,10 +13730,10 @@
         <v>17.94</v>
       </c>
       <c r="AI56" s="7">
-        <v>-392.60000000009</v>
+        <v>-95695.6</v>
       </c>
       <c r="AJ56" s="1">
-        <v>8347628.1</v>
+        <v>8023064.1</v>
       </c>
       <c r="AK56" s="2"/>
       <c r="AL56" s="1">
@@ -13769,10 +13769,10 @@
         <v>0.1</v>
       </c>
       <c r="G57" s="16">
-        <v>164582.0</v>
+        <v>276887.0</v>
       </c>
       <c r="H57" s="17">
-        <v>0.22000029407872</v>
+        <v>0.37012079951985</v>
       </c>
       <c r="I57" s="16">
         <v>0</v>
@@ -13819,26 +13819,26 @@
       </c>
       <c r="Z57" s="18"/>
       <c r="AA57" s="16">
-        <v>9628034.5</v>
+        <v>6164737.5</v>
       </c>
       <c r="AB57" s="16">
-        <v>12343633.5</v>
+        <v>0</v>
       </c>
       <c r="AC57" s="16">
-        <v>2715599.0</v>
+        <v>6178896.0</v>
       </c>
       <c r="AD57" s="17"/>
       <c r="AE57" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF57" s="17"/>
       <c r="AG57" s="17"/>
       <c r="AH57" s="17"/>
       <c r="AI57" s="16">
-        <v>-432.30000000005</v>
+        <v>-112737.3</v>
       </c>
       <c r="AJ57" s="16">
-        <v>8347195.8</v>
+        <v>7910326.8</v>
       </c>
       <c r="AK57" s="17"/>
       <c r="AL57" s="16">
@@ -13874,10 +13874,10 @@
         <v>0.09</v>
       </c>
       <c r="G58" s="1">
-        <v>181040.0</v>
+        <v>312049.0</v>
       </c>
       <c r="H58" s="2">
-        <v>0.22000002430402</v>
+        <v>0.37920231763172</v>
       </c>
       <c r="I58" s="1">
         <v>0</v>
@@ -13924,26 +13924,26 @@
       </c>
       <c r="Z58" s="3"/>
       <c r="AA58" s="1">
-        <v>9884782.5</v>
+        <v>6326027.5</v>
       </c>
       <c r="AB58" s="1">
-        <v>12672797.5</v>
+        <v>0</v>
       </c>
       <c r="AC58" s="6">
-        <v>2788015.0</v>
+        <v>6346770.0</v>
       </c>
       <c r="AD58" s="2"/>
       <c r="AE58" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF58" s="2"/>
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="7">
-        <v>-474.80000000005</v>
+        <v>-131483.8</v>
       </c>
       <c r="AJ58" s="1">
-        <v>8346721.0</v>
+        <v>7778843.0</v>
       </c>
       <c r="AK58" s="2"/>
       <c r="AL58" s="1">
@@ -13979,10 +13979,10 @@
         <v>0.1</v>
       </c>
       <c r="G59" s="1">
-        <v>199144.0</v>
+        <v>350725.0</v>
       </c>
       <c r="H59" s="2">
-        <v>0.22</v>
+        <v>0.38745581087053</v>
       </c>
       <c r="I59" s="1">
         <v>0</v>
@@ -14029,26 +14029,26 @@
       </c>
       <c r="Z59" s="3"/>
       <c r="AA59" s="1">
-        <v>10096598.8</v>
+        <v>6459090.8</v>
       </c>
       <c r="AB59" s="1">
-        <v>12944357.8</v>
+        <v>0</v>
       </c>
       <c r="AC59" s="6">
-        <v>2847759.0</v>
+        <v>6485267.0</v>
       </c>
       <c r="AD59" s="2"/>
       <c r="AE59" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF59" s="2"/>
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
       <c r="AI59" s="7">
-        <v>-522.30000000005</v>
+        <v>-152103.3</v>
       </c>
       <c r="AJ59" s="1">
-        <v>8346198.7</v>
+        <v>7626739.7</v>
       </c>
       <c r="AK59" s="2"/>
       <c r="AL59" s="1">
@@ -14084,10 +14084,10 @@
         <v>0.09</v>
       </c>
       <c r="G60" s="1">
-        <v>219058.0</v>
+        <v>395003.0</v>
       </c>
       <c r="H60" s="2">
-        <v>0.21999959828064</v>
+        <v>0.3967008797654</v>
       </c>
       <c r="I60" s="1">
         <v>0</v>
@@ -14134,26 +14134,26 @@
       </c>
       <c r="Z60" s="3"/>
       <c r="AA60" s="1">
-        <v>10251931.8</v>
+        <v>6556672.8</v>
       </c>
       <c r="AB60" s="1">
-        <v>13143501.8</v>
+        <v>0</v>
       </c>
       <c r="AC60" s="6">
-        <v>2891570.0</v>
+        <v>6586829.0</v>
       </c>
       <c r="AD60" s="2"/>
       <c r="AE60" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF60" s="2"/>
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="7">
-        <v>-573.80000000005</v>
+        <v>-176518.8</v>
       </c>
       <c r="AJ60" s="1">
-        <v>8345624.9</v>
+        <v>7450220.9</v>
       </c>
       <c r="AK60" s="2"/>
       <c r="AL60" s="1">
@@ -14189,10 +14189,10 @@
         <v>0.1</v>
       </c>
       <c r="G61" s="1">
-        <v>240964.0</v>
+        <v>444789.0</v>
       </c>
       <c r="H61" s="2">
-        <v>0.21999978088035</v>
+        <v>0.40609170887763</v>
       </c>
       <c r="I61" s="1">
         <v>0</v>
@@ -14239,26 +14239,26 @@
       </c>
       <c r="Z61" s="3"/>
       <c r="AA61" s="1">
-        <v>10337364.0</v>
+        <v>6610341.0</v>
       </c>
       <c r="AB61" s="1">
-        <v>13253031.0</v>
+        <v>0</v>
       </c>
       <c r="AC61" s="6">
-        <v>2915667.0</v>
+        <v>6642690.0</v>
       </c>
       <c r="AD61" s="2"/>
       <c r="AE61" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF61" s="2"/>
       <c r="AG61" s="2"/>
       <c r="AH61" s="2"/>
       <c r="AI61" s="7">
-        <v>-631.60000000009</v>
+        <v>-204456.6</v>
       </c>
       <c r="AJ61" s="1">
-        <v>8344993.3</v>
+        <v>7245764.3</v>
       </c>
       <c r="AK61" s="2"/>
       <c r="AL61" s="1">
@@ -14294,10 +14294,10 @@
         <v>0.1</v>
       </c>
       <c r="G62" s="1">
-        <v>265061.0</v>
+        <v>499555.0</v>
       </c>
       <c r="H62" s="2">
-        <v>0.22000031539955</v>
+        <v>0.41463005707902</v>
       </c>
       <c r="I62" s="1">
         <v>0</v>
@@ -14342,26 +14342,26 @@
       </c>
       <c r="Z62" s="3"/>
       <c r="AA62" s="1">
-        <v>10337364.0</v>
+        <v>6610341.0</v>
       </c>
       <c r="AB62" s="1">
-        <v>13253031.0</v>
+        <v>0</v>
       </c>
       <c r="AC62" s="6">
-        <v>2915667.0</v>
+        <v>6642690.0</v>
       </c>
       <c r="AD62" s="2"/>
       <c r="AE62" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF62" s="2"/>
       <c r="AG62" s="2"/>
       <c r="AH62" s="2"/>
       <c r="AI62" s="7">
-        <v>-696.20000000019</v>
+        <v>-235190.2</v>
       </c>
       <c r="AJ62" s="1">
-        <v>8344297.1</v>
+        <v>7010574.1</v>
       </c>
       <c r="AK62" s="2"/>
       <c r="AL62" s="1">
@@ -14397,10 +14397,10 @@
         <v>0.09</v>
       </c>
       <c r="G63" s="1">
-        <v>291567.0</v>
+        <v>559796.0</v>
       </c>
       <c r="H63" s="2">
-        <v>0.22000025654511</v>
+        <v>0.42239095512498</v>
       </c>
       <c r="I63" s="1">
         <v>0</v>
@@ -14447,26 +14447,26 @@
       </c>
       <c r="Z63" s="3"/>
       <c r="AA63" s="1">
-        <v>10233990.8</v>
+        <v>6545401.8</v>
       </c>
       <c r="AB63" s="1">
-        <v>13120500.8</v>
+        <v>0</v>
       </c>
       <c r="AC63" s="6">
-        <v>2886510.0</v>
+        <v>6575099.0</v>
       </c>
       <c r="AD63" s="2"/>
       <c r="AE63" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF63" s="2"/>
       <c r="AG63" s="2"/>
       <c r="AH63" s="2"/>
       <c r="AI63" s="7">
-        <v>-765.70000000019</v>
+        <v>-268994.7</v>
       </c>
       <c r="AJ63" s="1">
-        <v>8343531.4</v>
+        <v>6741579.4</v>
       </c>
       <c r="AK63" s="2"/>
       <c r="AL63" s="1">
@@ -14502,10 +14502,10 @@
         <v>0.1</v>
       </c>
       <c r="G64" s="1">
-        <v>320723.0</v>
+        <v>627139.0</v>
       </c>
       <c r="H64" s="2">
-        <v>0.2199998216531</v>
+        <v>0.43018576201801</v>
       </c>
       <c r="I64" s="1">
         <v>0</v>
@@ -14552,26 +14552,26 @@
       </c>
       <c r="Z64" s="3"/>
       <c r="AA64" s="1">
-        <v>10006568.8</v>
+        <v>6402535.8</v>
       </c>
       <c r="AB64" s="1">
-        <v>12828934.8</v>
+        <v>0</v>
       </c>
       <c r="AC64" s="6">
-        <v>2822366.0</v>
+        <v>6426399.0</v>
       </c>
       <c r="AD64" s="2"/>
       <c r="AE64" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF64" s="2"/>
       <c r="AG64" s="2"/>
       <c r="AH64" s="2"/>
       <c r="AI64" s="7">
-        <v>-842.5</v>
+        <v>-307258.5</v>
       </c>
       <c r="AJ64" s="1">
-        <v>8342688.9</v>
+        <v>6434320.9</v>
       </c>
       <c r="AK64" s="2"/>
       <c r="AL64" s="1">
@@ -14607,10 +14607,10 @@
         <v>0.1</v>
       </c>
       <c r="G65" s="1">
-        <v>352796.0</v>
+        <v>701489.0</v>
       </c>
       <c r="H65" s="2">
-        <v>0.22000016213348</v>
+        <v>0.4374417332817</v>
       </c>
       <c r="I65" s="1">
         <v>0</v>
@@ -14657,26 +14657,26 @@
       </c>
       <c r="Z65" s="3"/>
       <c r="AA65" s="1">
-        <v>9631322.8</v>
+        <v>6166802.8</v>
       </c>
       <c r="AB65" s="1">
-        <v>12347849.8</v>
+        <v>0</v>
       </c>
       <c r="AC65" s="6">
-        <v>2716527.0</v>
+        <v>6181047.0</v>
       </c>
       <c r="AD65" s="2"/>
       <c r="AE65" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF65" s="2"/>
       <c r="AG65" s="2"/>
       <c r="AH65" s="2"/>
       <c r="AI65" s="7">
-        <v>-926.60000000009</v>
+        <v>-349619.6</v>
       </c>
       <c r="AJ65" s="1">
-        <v>8341762.3</v>
+        <v>6084701.3</v>
       </c>
       <c r="AK65" s="2"/>
       <c r="AL65" s="1">
@@ -14712,10 +14712,10 @@
         <v>0.1</v>
       </c>
       <c r="G66" s="1">
-        <v>388075.0</v>
+        <v>783273.0</v>
       </c>
       <c r="H66" s="2">
-        <v>0.21999978457793</v>
+        <v>0.44403759908706</v>
       </c>
       <c r="I66" s="1">
         <v>0</v>
@@ -14762,26 +14762,26 @@
       </c>
       <c r="Z66" s="3"/>
       <c r="AA66" s="1">
-        <v>9080961.1</v>
+        <v>5821063.1</v>
       </c>
       <c r="AB66" s="1">
-        <v>11642258.1</v>
+        <v>0</v>
       </c>
       <c r="AC66" s="6">
-        <v>2561297.0</v>
+        <v>5821195.0</v>
       </c>
       <c r="AD66" s="2"/>
       <c r="AE66" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF66" s="2"/>
       <c r="AG66" s="2"/>
       <c r="AH66" s="2"/>
       <c r="AI66" s="7">
-        <v>-1018.5000000005</v>
+        <v>-396216.5</v>
       </c>
       <c r="AJ66" s="1">
-        <v>8340743.8</v>
+        <v>5688484.8</v>
       </c>
       <c r="AK66" s="2"/>
       <c r="AL66" s="1">
@@ -14817,10 +14817,10 @@
         <v>0.1</v>
       </c>
       <c r="G67" s="1">
-        <v>426883.0</v>
+        <v>873236.0</v>
       </c>
       <c r="H67" s="2">
-        <v>0.22000014430193</v>
+        <v>0.45003442631737</v>
       </c>
       <c r="I67" s="1">
         <v>0</v>
@@ -14867,26 +14867,26 @@
       </c>
       <c r="Z67" s="3"/>
       <c r="AA67" s="1">
-        <v>8324215.2</v>
+        <v>5345671.2</v>
       </c>
       <c r="AB67" s="1">
-        <v>10672070.2</v>
+        <v>0</v>
       </c>
       <c r="AC67" s="6">
-        <v>2347855.0</v>
+        <v>5326399.0</v>
       </c>
       <c r="AD67" s="2"/>
       <c r="AE67" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF67" s="2"/>
       <c r="AG67" s="2"/>
       <c r="AH67" s="2"/>
       <c r="AI67" s="7">
-        <v>-1123.2000000002</v>
+        <v>-447476.2</v>
       </c>
       <c r="AJ67" s="1">
-        <v>8339620.6</v>
+        <v>5241008.6</v>
       </c>
       <c r="AK67" s="2"/>
       <c r="AL67" s="1">
@@ -14922,10 +14922,10 @@
         <v>0.09</v>
       </c>
       <c r="G68" s="1">
-        <v>469571.0</v>
+        <v>972195.0</v>
       </c>
       <c r="H68" s="2">
-        <v>0.21999996251899</v>
+        <v>0.45548567428812</v>
       </c>
       <c r="I68" s="1">
         <v>0</v>
@@ -14972,26 +14972,26 @@
       </c>
       <c r="Z68" s="3"/>
       <c r="AA68" s="1">
-        <v>7325308.6</v>
+        <v>4718152.6</v>
       </c>
       <c r="AB68" s="1">
-        <v>9391421.6</v>
+        <v>0</v>
       </c>
       <c r="AC68" s="6">
-        <v>2066113.0</v>
+        <v>4673269.0</v>
       </c>
       <c r="AD68" s="2"/>
       <c r="AE68" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF68" s="2"/>
       <c r="AG68" s="2"/>
       <c r="AH68" s="2"/>
       <c r="AI68" s="7">
-        <v>-1234.2000000002</v>
+        <v>-503858.2</v>
       </c>
       <c r="AJ68" s="1">
-        <v>8338386.4</v>
+        <v>4737150.4</v>
       </c>
       <c r="AK68" s="2"/>
       <c r="AL68" s="1">
@@ -15027,10 +15027,10 @@
         <v>0.09</v>
       </c>
       <c r="G69" s="1">
-        <v>516528.0</v>
+        <v>1081051.0</v>
       </c>
       <c r="H69" s="2">
-        <v>0.21999986370544</v>
+        <v>0.46044178177878</v>
       </c>
       <c r="I69" s="1">
         <v>0</v>
@@ -15077,26 +15077,26 @@
       </c>
       <c r="Z69" s="3"/>
       <c r="AA69" s="1">
-        <v>6043379.6</v>
+        <v>3912838.6</v>
       </c>
       <c r="AB69" s="1">
-        <v>7747922.6</v>
+        <v>0</v>
       </c>
       <c r="AC69" s="6">
-        <v>1704543.0</v>
+        <v>3835084.0</v>
       </c>
       <c r="AD69" s="2"/>
       <c r="AE69" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF69" s="2"/>
       <c r="AG69" s="2"/>
       <c r="AH69" s="2"/>
       <c r="AI69" s="7">
-        <v>-1356.1000000006</v>
+        <v>-565879.1</v>
       </c>
       <c r="AJ69" s="1">
-        <v>8337030.3</v>
+        <v>4171271.3</v>
       </c>
       <c r="AK69" s="2"/>
       <c r="AL69" s="1">
@@ -15132,10 +15132,10 @@
         <v>0.09</v>
       </c>
       <c r="G70" s="1">
-        <v>568181.0</v>
+        <v>1200791.0</v>
       </c>
       <c r="H70" s="2">
-        <v>0.21999999225599</v>
+        <v>0.46494692835744</v>
       </c>
       <c r="I70" s="1">
         <v>0</v>
@@ -15182,26 +15182,26 @@
       </c>
       <c r="Z70" s="3"/>
       <c r="AA70" s="1">
-        <v>4431812.2</v>
+        <v>2900443.2</v>
       </c>
       <c r="AB70" s="1">
-        <v>5681810.2</v>
+        <v>0</v>
       </c>
       <c r="AC70" s="6">
-        <v>1249998.0</v>
+        <v>2781367.0</v>
       </c>
       <c r="AD70" s="2"/>
       <c r="AE70" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF70" s="2"/>
       <c r="AG70" s="2"/>
       <c r="AH70" s="2"/>
       <c r="AI70" s="7">
-        <v>-1493.0</v>
+        <v>-634103.0</v>
       </c>
       <c r="AJ70" s="1">
-        <v>8335537.3</v>
+        <v>3537168.3</v>
       </c>
       <c r="AK70" s="2"/>
       <c r="AL70" s="1">
@@ -15237,10 +15237,10 @@
         <v>0.1</v>
       </c>
       <c r="G71" s="1">
-        <v>624999.0</v>
+        <v>1332505.0</v>
       </c>
       <c r="H71" s="2">
-        <v>0.21999996479995</v>
+        <v>0.46904243542111</v>
       </c>
       <c r="I71" s="1">
         <v>0</v>
@@ -15287,26 +15287,26 @@
       </c>
       <c r="Z71" s="3"/>
       <c r="AA71" s="1">
-        <v>2437496.5</v>
+        <v>1647604.5</v>
       </c>
       <c r="AB71" s="1">
-        <v>3124995.5</v>
+        <v>0</v>
       </c>
       <c r="AC71" s="6">
-        <v>687499.0</v>
+        <v>1477391.0</v>
       </c>
       <c r="AD71" s="2"/>
       <c r="AE71" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF71" s="2"/>
       <c r="AG71" s="2"/>
       <c r="AH71" s="2"/>
       <c r="AI71" s="7">
-        <v>-1642.4000000004</v>
+        <v>-709148.4</v>
       </c>
       <c r="AJ71" s="1">
-        <v>8333894.9</v>
+        <v>2828019.9</v>
       </c>
       <c r="AK71" s="2"/>
       <c r="AL71" s="1">
@@ -15342,10 +15342,10 @@
         <v>0.09</v>
       </c>
       <c r="G72" s="6">
-        <v>687499.0</v>
+        <v>1477392.0</v>
       </c>
       <c r="H72" s="20">
-        <v>0.21999996159995</v>
+        <v>0.47276604514054</v>
       </c>
       <c r="I72" s="6">
         <v>0</v>
@@ -15406,10 +15406,10 @@
       <c r="AG72" s="20"/>
       <c r="AH72" s="20"/>
       <c r="AI72" s="6">
-        <v>-1805.3000000007</v>
+        <v>-791698.3</v>
       </c>
       <c r="AJ72" s="6">
-        <v>8332089.6</v>
+        <v>2036321.6</v>
       </c>
       <c r="AK72" s="20"/>
       <c r="AL72" s="6">
@@ -28368,19 +28368,17 @@
       <c r="Y37" s="6"/>
       <c r="Z37" s="3"/>
       <c r="AA37" s="1">
-        <v>1233452.0</v>
+        <v>736181.0</v>
       </c>
       <c r="AB37" s="1">
-        <v>150900.0</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="6">
-        <v>33198.0</v>
-      </c>
-      <c r="AD37" s="2">
-        <v>0.22</v>
-      </c>
+        <v>530469.0</v>
+      </c>
+      <c r="AD37" s="2"/>
       <c r="AE37" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
@@ -28455,19 +28453,17 @@
       <c r="Y38" s="6"/>
       <c r="Z38" s="3"/>
       <c r="AA38" s="1">
-        <v>1154267.0</v>
+        <v>841472.0</v>
       </c>
       <c r="AB38" s="1">
-        <v>1479830.0</v>
+        <v>0</v>
       </c>
       <c r="AC38" s="6">
-        <v>325563.0</v>
-      </c>
-      <c r="AD38" s="2">
-        <v>0.22</v>
-      </c>
+        <v>638358.0</v>
+      </c>
+      <c r="AD38" s="2"/>
       <c r="AE38" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
@@ -28542,19 +28538,17 @@
       <c r="Y39" s="9"/>
       <c r="Z39" s="11"/>
       <c r="AA39" s="9">
-        <v>1343924.6</v>
+        <v>960616.6</v>
       </c>
       <c r="AB39" s="9">
-        <v>1722980.6</v>
+        <v>0</v>
       </c>
       <c r="AC39" s="9">
-        <v>379056.0</v>
-      </c>
-      <c r="AD39" s="10">
-        <v>0.22</v>
-      </c>
+        <v>762364.0</v>
+      </c>
+      <c r="AD39" s="10"/>
       <c r="AE39" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF39" s="10"/>
       <c r="AG39" s="10"/>
@@ -28631,19 +28625,17 @@
       <c r="Y40" s="13"/>
       <c r="Z40" s="15"/>
       <c r="AA40" s="13">
-        <v>1559969.7</v>
+        <v>1096337.7</v>
       </c>
       <c r="AB40" s="13">
-        <v>1999961.7</v>
+        <v>0</v>
       </c>
       <c r="AC40" s="13">
-        <v>439992.0</v>
-      </c>
-      <c r="AD40" s="14">
-        <v>0.22</v>
-      </c>
+        <v>903624.0</v>
+      </c>
+      <c r="AD40" s="14"/>
       <c r="AE40" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF40" s="14"/>
       <c r="AG40" s="14"/>
@@ -28720,19 +28712,17 @@
       <c r="Y41" s="6"/>
       <c r="Z41" s="3"/>
       <c r="AA41" s="1">
-        <v>1805786.6</v>
+        <v>1250760.6</v>
       </c>
       <c r="AB41" s="1">
-        <v>2315110.6</v>
+        <v>0</v>
       </c>
       <c r="AC41" s="6">
-        <v>509324.0</v>
-      </c>
-      <c r="AD41" s="2">
-        <v>0.22</v>
-      </c>
+        <v>1064350.0</v>
+      </c>
+      <c r="AD41" s="2"/>
       <c r="AE41" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
@@ -28809,19 +28799,17 @@
       <c r="Y42" s="6"/>
       <c r="Z42" s="3"/>
       <c r="AA42" s="1">
-        <v>2085165.3</v>
+        <v>1426267.3</v>
       </c>
       <c r="AB42" s="1">
-        <v>2673289.3</v>
+        <v>0</v>
       </c>
       <c r="AC42" s="6">
-        <v>588124.0</v>
-      </c>
-      <c r="AD42" s="2">
-        <v>0.22</v>
-      </c>
+        <v>1247022.0</v>
+      </c>
+      <c r="AD42" s="2"/>
       <c r="AE42" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
@@ -28898,19 +28886,17 @@
       <c r="Y43" s="6"/>
       <c r="Z43" s="3"/>
       <c r="AA43" s="1">
-        <v>2402361.5</v>
+        <v>1625532.5</v>
       </c>
       <c r="AB43" s="1">
-        <v>3079950.5</v>
+        <v>0</v>
       </c>
       <c r="AC43" s="6">
-        <v>677589.0</v>
-      </c>
-      <c r="AD43" s="2">
-        <v>0.22</v>
-      </c>
+        <v>1454418.0</v>
+      </c>
+      <c r="AD43" s="2"/>
       <c r="AE43" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
@@ -28987,19 +28973,17 @@
       <c r="Y44" s="6"/>
       <c r="Z44" s="3"/>
       <c r="AA44" s="1">
-        <v>2762146.5</v>
+        <v>1851551.5</v>
       </c>
       <c r="AB44" s="1">
-        <v>3541213.5</v>
+        <v>0</v>
       </c>
       <c r="AC44" s="6">
-        <v>779067.0</v>
-      </c>
-      <c r="AD44" s="2">
-        <v>0.22</v>
-      </c>
+        <v>1689662.0</v>
+      </c>
+      <c r="AD44" s="2"/>
       <c r="AE44" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF44" s="2"/>
       <c r="AG44" s="2"/>
@@ -29076,19 +29060,17 @@
       <c r="Y45" s="6"/>
       <c r="Z45" s="3"/>
       <c r="AA45" s="1">
-        <v>3169864.0</v>
+        <v>2107681.0</v>
       </c>
       <c r="AB45" s="1">
-        <v>4063928.0</v>
+        <v>0</v>
       </c>
       <c r="AC45" s="6">
-        <v>894064.0</v>
-      </c>
-      <c r="AD45" s="2">
-        <v>0.22</v>
-      </c>
+        <v>1956247.0</v>
+      </c>
+      <c r="AD45" s="2"/>
       <c r="AE45" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF45" s="2"/>
       <c r="AG45" s="2"/>
@@ -29165,19 +29147,17 @@
       <c r="Y46" s="6"/>
       <c r="Z46" s="3"/>
       <c r="AA46" s="1">
-        <v>3631504.2</v>
+        <v>2397686.2</v>
       </c>
       <c r="AB46" s="1">
-        <v>4655774.2</v>
+        <v>0</v>
       </c>
       <c r="AC46" s="6">
-        <v>1024270.0</v>
-      </c>
-      <c r="AD46" s="2">
-        <v>0.22</v>
-      </c>
+        <v>2258088.0</v>
+      </c>
+      <c r="AD46" s="2"/>
       <c r="AE46" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF46" s="2"/>
       <c r="AG46" s="2"/>
@@ -29254,19 +29234,17 @@
       <c r="Y47" s="6"/>
       <c r="Z47" s="3"/>
       <c r="AA47" s="1">
-        <v>4153771.6</v>
+        <v>2725776.6</v>
       </c>
       <c r="AB47" s="1">
-        <v>5325348.6</v>
+        <v>0</v>
       </c>
       <c r="AC47" s="6">
-        <v>1171577.0</v>
-      </c>
-      <c r="AD47" s="2">
-        <v>0.22</v>
-      </c>
+        <v>2599572.0</v>
+      </c>
+      <c r="AD47" s="2"/>
       <c r="AE47" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF47" s="2"/>
       <c r="AG47" s="2"/>
@@ -29343,19 +29321,17 @@
       <c r="Y48" s="6"/>
       <c r="Z48" s="3"/>
       <c r="AA48" s="1">
-        <v>4744179.7</v>
+        <v>3096674.7</v>
       </c>
       <c r="AB48" s="1">
-        <v>6082281.7</v>
+        <v>0</v>
       </c>
       <c r="AC48" s="6">
-        <v>1338102.0</v>
-      </c>
-      <c r="AD48" s="2">
-        <v>0.22</v>
-      </c>
+        <v>2985607.0</v>
+      </c>
+      <c r="AD48" s="2"/>
       <c r="AE48" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF48" s="2"/>
       <c r="AG48" s="2"/>
@@ -29432,19 +29408,17 @@
       <c r="Y49" s="6"/>
       <c r="Z49" s="3"/>
       <c r="AA49" s="1">
-        <v>5411131.0</v>
+        <v>3515656.0</v>
       </c>
       <c r="AB49" s="1">
-        <v>6937348.0</v>
+        <v>0</v>
       </c>
       <c r="AC49" s="6">
-        <v>1526217.0</v>
-      </c>
-      <c r="AD49" s="2">
-        <v>0.22</v>
-      </c>
+        <v>3421692.0</v>
+      </c>
+      <c r="AD49" s="2"/>
       <c r="AE49" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF49" s="2"/>
       <c r="AG49" s="2"/>
@@ -29521,19 +29495,17 @@
       <c r="Y50" s="6"/>
       <c r="Z50" s="3"/>
       <c r="AA50" s="1">
-        <v>6164031.6</v>
+        <v>3988632.6</v>
       </c>
       <c r="AB50" s="1">
-        <v>7902604.6</v>
+        <v>0</v>
       </c>
       <c r="AC50" s="6">
-        <v>1738573.0</v>
-      </c>
-      <c r="AD50" s="2">
-        <v>0.22</v>
-      </c>
+        <v>3913972.0</v>
+      </c>
+      <c r="AD50" s="2"/>
       <c r="AE50" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF50" s="2"/>
       <c r="AG50" s="2"/>
@@ -29610,19 +29582,17 @@
       <c r="Y51" s="6"/>
       <c r="Z51" s="3"/>
       <c r="AA51" s="1">
-        <v>7013400.7</v>
+        <v>4522210.7</v>
       </c>
       <c r="AB51" s="1">
-        <v>8991539.7</v>
+        <v>0</v>
       </c>
       <c r="AC51" s="6">
-        <v>1978139.0</v>
-      </c>
-      <c r="AD51" s="2">
-        <v>0.22</v>
-      </c>
+        <v>4469329.0</v>
+      </c>
+      <c r="AD51" s="2"/>
       <c r="AE51" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF51" s="2"/>
       <c r="AG51" s="2"/>
@@ -29699,19 +29669,17 @@
       <c r="Y52" s="6"/>
       <c r="Z52" s="3"/>
       <c r="AA52" s="1">
-        <v>7971003.4</v>
+        <v>5123781.4</v>
       </c>
       <c r="AB52" s="1">
-        <v>10219235.4</v>
+        <v>0</v>
       </c>
       <c r="AC52" s="6">
-        <v>2248232.0</v>
-      </c>
-      <c r="AD52" s="2">
-        <v>0.22</v>
-      </c>
+        <v>5095454.0</v>
+      </c>
+      <c r="AD52" s="2"/>
       <c r="AE52" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF52" s="2"/>
       <c r="AG52" s="2"/>
@@ -29788,19 +29756,17 @@
       <c r="Y53" s="16"/>
       <c r="Z53" s="18"/>
       <c r="AA53" s="16">
-        <v>8329698.3</v>
+        <v>5349115.3</v>
       </c>
       <c r="AB53" s="16">
-        <v>10679100.3</v>
+        <v>0</v>
       </c>
       <c r="AC53" s="16">
-        <v>2349402.0</v>
-      </c>
-      <c r="AD53" s="17">
-        <v>0.22</v>
-      </c>
+        <v>5329985.0</v>
+      </c>
+      <c r="AD53" s="17"/>
       <c r="AE53" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF53" s="17"/>
       <c r="AG53" s="17"/>
@@ -29875,19 +29841,17 @@
       <c r="Y54" s="6"/>
       <c r="Z54" s="3"/>
       <c r="AA54" s="1">
-        <v>8680422.2</v>
+        <v>5569442.2</v>
       </c>
       <c r="AB54" s="1">
-        <v>11128746.2</v>
+        <v>0</v>
       </c>
       <c r="AC54" s="6">
-        <v>2448324.0</v>
-      </c>
-      <c r="AD54" s="2">
-        <v>0.22</v>
-      </c>
+        <v>5559304.0</v>
+      </c>
+      <c r="AD54" s="2"/>
       <c r="AE54" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF54" s="2"/>
       <c r="AG54" s="2"/>
@@ -29962,19 +29926,17 @@
       <c r="Y55" s="6"/>
       <c r="Z55" s="3"/>
       <c r="AA55" s="1">
-        <v>9017993.2</v>
+        <v>5781506.2</v>
       </c>
       <c r="AB55" s="1">
-        <v>11561530.2</v>
+        <v>0</v>
       </c>
       <c r="AC55" s="6">
-        <v>2543537.0</v>
-      </c>
-      <c r="AD55" s="2">
-        <v>0.22</v>
-      </c>
+        <v>5780024.0</v>
+      </c>
+      <c r="AD55" s="2"/>
       <c r="AE55" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF55" s="2"/>
       <c r="AG55" s="2"/>
@@ -30049,19 +30011,17 @@
       <c r="Y56" s="6"/>
       <c r="Z56" s="3"/>
       <c r="AA56" s="1">
-        <v>9336276.0</v>
+        <v>5981452.0</v>
       </c>
       <c r="AB56" s="1">
-        <v>11969584.0</v>
+        <v>0</v>
       </c>
       <c r="AC56" s="6">
-        <v>2633308.0</v>
-      </c>
-      <c r="AD56" s="2">
-        <v>0.22</v>
-      </c>
+        <v>5988132.0</v>
+      </c>
+      <c r="AD56" s="2"/>
       <c r="AE56" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF56" s="2"/>
       <c r="AG56" s="2"/>
@@ -30136,19 +30096,17 @@
       <c r="Y57" s="16"/>
       <c r="Z57" s="18"/>
       <c r="AA57" s="16">
-        <v>9628034.5</v>
+        <v>6164737.5</v>
       </c>
       <c r="AB57" s="16">
-        <v>12343633.5</v>
+        <v>0</v>
       </c>
       <c r="AC57" s="16">
-        <v>2715599.0</v>
-      </c>
-      <c r="AD57" s="17">
-        <v>0.22</v>
-      </c>
+        <v>6178896.0</v>
+      </c>
+      <c r="AD57" s="17"/>
       <c r="AE57" s="16">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF57" s="17"/>
       <c r="AG57" s="17"/>
@@ -30223,19 +30181,17 @@
       <c r="Y58" s="6"/>
       <c r="Z58" s="3"/>
       <c r="AA58" s="1">
-        <v>9884782.5</v>
+        <v>6326027.5</v>
       </c>
       <c r="AB58" s="1">
-        <v>12672797.5</v>
+        <v>0</v>
       </c>
       <c r="AC58" s="6">
-        <v>2788015.0</v>
-      </c>
-      <c r="AD58" s="2">
-        <v>0.22</v>
-      </c>
+        <v>6346770.0</v>
+      </c>
+      <c r="AD58" s="2"/>
       <c r="AE58" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF58" s="2"/>
       <c r="AG58" s="2"/>
@@ -30310,19 +30266,17 @@
       <c r="Y59" s="6"/>
       <c r="Z59" s="3"/>
       <c r="AA59" s="1">
-        <v>10096598.8</v>
+        <v>6459090.8</v>
       </c>
       <c r="AB59" s="1">
-        <v>12944357.8</v>
+        <v>0</v>
       </c>
       <c r="AC59" s="6">
-        <v>2847759.0</v>
-      </c>
-      <c r="AD59" s="2">
-        <v>0.22</v>
-      </c>
+        <v>6485267.0</v>
+      </c>
+      <c r="AD59" s="2"/>
       <c r="AE59" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF59" s="2"/>
       <c r="AG59" s="2"/>
@@ -30397,19 +30351,17 @@
       <c r="Y60" s="6"/>
       <c r="Z60" s="3"/>
       <c r="AA60" s="1">
-        <v>10251931.8</v>
+        <v>6556672.8</v>
       </c>
       <c r="AB60" s="1">
-        <v>13143501.8</v>
+        <v>0</v>
       </c>
       <c r="AC60" s="6">
-        <v>2891570.0</v>
-      </c>
-      <c r="AD60" s="2">
-        <v>0.22</v>
-      </c>
+        <v>6586829.0</v>
+      </c>
+      <c r="AD60" s="2"/>
       <c r="AE60" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF60" s="2"/>
       <c r="AG60" s="2"/>
@@ -30484,19 +30436,17 @@
       <c r="Y61" s="6"/>
       <c r="Z61" s="3"/>
       <c r="AA61" s="1">
-        <v>10337364.0</v>
+        <v>6610341.0</v>
       </c>
       <c r="AB61" s="1">
-        <v>13253031.0</v>
+        <v>0</v>
       </c>
       <c r="AC61" s="6">
-        <v>2915667.0</v>
-      </c>
-      <c r="AD61" s="2">
-        <v>0.22</v>
-      </c>
+        <v>6642690.0</v>
+      </c>
+      <c r="AD61" s="2"/>
       <c r="AE61" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF61" s="2"/>
       <c r="AG61" s="2"/>
@@ -30571,19 +30521,17 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="3"/>
       <c r="AA62" s="1">
-        <v>10337364.0</v>
+        <v>6610341.0</v>
       </c>
       <c r="AB62" s="1">
-        <v>13253031.0</v>
+        <v>0</v>
       </c>
       <c r="AC62" s="6">
-        <v>2915667.0</v>
-      </c>
-      <c r="AD62" s="2">
-        <v>0.22</v>
-      </c>
+        <v>6642690.0</v>
+      </c>
+      <c r="AD62" s="2"/>
       <c r="AE62" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF62" s="2"/>
       <c r="AG62" s="2"/>
@@ -30658,19 +30606,17 @@
       <c r="Y63" s="6"/>
       <c r="Z63" s="3"/>
       <c r="AA63" s="1">
-        <v>10233990.8</v>
+        <v>6545401.8</v>
       </c>
       <c r="AB63" s="1">
-        <v>13120500.8</v>
+        <v>0</v>
       </c>
       <c r="AC63" s="6">
-        <v>2886510.0</v>
-      </c>
-      <c r="AD63" s="2">
-        <v>0.22</v>
-      </c>
+        <v>6575099.0</v>
+      </c>
+      <c r="AD63" s="2"/>
       <c r="AE63" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF63" s="2"/>
       <c r="AG63" s="2"/>
@@ -30745,19 +30691,17 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="3"/>
       <c r="AA64" s="1">
-        <v>10006568.8</v>
+        <v>6402535.8</v>
       </c>
       <c r="AB64" s="1">
-        <v>12828934.8</v>
+        <v>0</v>
       </c>
       <c r="AC64" s="6">
-        <v>2822366.0</v>
-      </c>
-      <c r="AD64" s="2">
-        <v>0.22</v>
-      </c>
+        <v>6426399.0</v>
+      </c>
+      <c r="AD64" s="2"/>
       <c r="AE64" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF64" s="2"/>
       <c r="AG64" s="2"/>
@@ -30832,19 +30776,17 @@
       <c r="Y65" s="6"/>
       <c r="Z65" s="3"/>
       <c r="AA65" s="1">
-        <v>9631322.8</v>
+        <v>6166802.8</v>
       </c>
       <c r="AB65" s="1">
-        <v>12347849.8</v>
+        <v>0</v>
       </c>
       <c r="AC65" s="6">
-        <v>2716527.0</v>
-      </c>
-      <c r="AD65" s="2">
-        <v>0.22</v>
-      </c>
+        <v>6181047.0</v>
+      </c>
+      <c r="AD65" s="2"/>
       <c r="AE65" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF65" s="2"/>
       <c r="AG65" s="2"/>
@@ -30919,19 +30861,17 @@
       <c r="Y66" s="6"/>
       <c r="Z66" s="3"/>
       <c r="AA66" s="1">
-        <v>9080961.1</v>
+        <v>5821063.1</v>
       </c>
       <c r="AB66" s="1">
-        <v>11642258.1</v>
+        <v>0</v>
       </c>
       <c r="AC66" s="6">
-        <v>2561297.0</v>
-      </c>
-      <c r="AD66" s="2">
-        <v>0.22</v>
-      </c>
+        <v>5821195.0</v>
+      </c>
+      <c r="AD66" s="2"/>
       <c r="AE66" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF66" s="2"/>
       <c r="AG66" s="2"/>
@@ -31006,19 +30946,17 @@
       <c r="Y67" s="6"/>
       <c r="Z67" s="3"/>
       <c r="AA67" s="1">
-        <v>8324215.2</v>
+        <v>5345671.2</v>
       </c>
       <c r="AB67" s="1">
-        <v>10672070.2</v>
+        <v>0</v>
       </c>
       <c r="AC67" s="6">
-        <v>2347855.0</v>
-      </c>
-      <c r="AD67" s="2">
-        <v>0.22</v>
-      </c>
+        <v>5326399.0</v>
+      </c>
+      <c r="AD67" s="2"/>
       <c r="AE67" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF67" s="2"/>
       <c r="AG67" s="2"/>
@@ -31093,19 +31031,17 @@
       <c r="Y68" s="6"/>
       <c r="Z68" s="3"/>
       <c r="AA68" s="1">
-        <v>7325308.6</v>
+        <v>4718152.6</v>
       </c>
       <c r="AB68" s="1">
-        <v>9391421.6</v>
+        <v>0</v>
       </c>
       <c r="AC68" s="6">
-        <v>2066113.0</v>
-      </c>
-      <c r="AD68" s="2">
-        <v>0.22</v>
-      </c>
+        <v>4673269.0</v>
+      </c>
+      <c r="AD68" s="2"/>
       <c r="AE68" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF68" s="2"/>
       <c r="AG68" s="2"/>
@@ -31180,19 +31116,17 @@
       <c r="Y69" s="6"/>
       <c r="Z69" s="3"/>
       <c r="AA69" s="1">
-        <v>6043379.6</v>
+        <v>3912838.6</v>
       </c>
       <c r="AB69" s="1">
-        <v>7747922.6</v>
+        <v>0</v>
       </c>
       <c r="AC69" s="6">
-        <v>1704543.0</v>
-      </c>
-      <c r="AD69" s="2">
-        <v>0.22</v>
-      </c>
+        <v>3835084.0</v>
+      </c>
+      <c r="AD69" s="2"/>
       <c r="AE69" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF69" s="2"/>
       <c r="AG69" s="2"/>
@@ -31267,19 +31201,17 @@
       <c r="Y70" s="6"/>
       <c r="Z70" s="3"/>
       <c r="AA70" s="1">
-        <v>4431812.2</v>
+        <v>2900443.2</v>
       </c>
       <c r="AB70" s="1">
-        <v>5681810.2</v>
+        <v>0</v>
       </c>
       <c r="AC70" s="6">
-        <v>1249998.0</v>
-      </c>
-      <c r="AD70" s="2">
-        <v>0.22</v>
-      </c>
+        <v>2781367.0</v>
+      </c>
+      <c r="AD70" s="2"/>
       <c r="AE70" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF70" s="2"/>
       <c r="AG70" s="2"/>
@@ -31354,19 +31286,17 @@
       <c r="Y71" s="6"/>
       <c r="Z71" s="3"/>
       <c r="AA71" s="1">
-        <v>2437496.5</v>
+        <v>1647604.5</v>
       </c>
       <c r="AB71" s="1">
-        <v>3124995.5</v>
+        <v>0</v>
       </c>
       <c r="AC71" s="6">
-        <v>687499.0</v>
-      </c>
-      <c r="AD71" s="2">
-        <v>0.22</v>
-      </c>
+        <v>1477391.0</v>
+      </c>
+      <c r="AD71" s="2"/>
       <c r="AE71" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="AF71" s="2"/>
       <c r="AG71" s="2"/>
@@ -31845,7 +31775,7 @@
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="238.228" bestFit="true" customWidth="true" style="0"/>
@@ -35375,7 +35305,7 @@
       <c r="E53" s="16"/>
       <c r="F53" s="17"/>
       <c r="G53" s="16">
-        <v>112412.0</v>
+        <v>180701.0</v>
       </c>
       <c r="H53" s="17">
         <v>0</v>
@@ -35417,10 +35347,10 @@
       <c r="AG53" s="17"/>
       <c r="AH53" s="17"/>
       <c r="AI53" s="16">
-        <v>909512.0</v>
+        <v>841223.0</v>
       </c>
       <c r="AJ53" s="16">
-        <v>909512.0</v>
+        <v>841223.0</v>
       </c>
       <c r="AK53" s="17"/>
       <c r="AL53" s="16">
@@ -35452,7 +35382,7 @@
       <c r="E54" s="6"/>
       <c r="F54" s="2"/>
       <c r="G54" s="1">
-        <v>123653.0</v>
+        <v>199811.0</v>
       </c>
       <c r="H54" s="2">
         <v>0</v>
@@ -35494,10 +35424,10 @@
       <c r="AG54" s="2"/>
       <c r="AH54" s="2"/>
       <c r="AI54" s="7">
-        <v>1000463.0</v>
+        <v>924305.0</v>
       </c>
       <c r="AJ54" s="1">
-        <v>1909975.0</v>
+        <v>1765528.0</v>
       </c>
       <c r="AK54" s="2"/>
       <c r="AL54" s="1">
@@ -35529,7 +35459,7 @@
       <c r="E55" s="6"/>
       <c r="F55" s="2"/>
       <c r="G55" s="1">
-        <v>136018.0</v>
+        <v>220832.0</v>
       </c>
       <c r="H55" s="2">
         <v>0</v>
@@ -35571,10 +35501,10 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="2"/>
       <c r="AI55" s="7">
-        <v>1100510.0</v>
+        <v>1015696.0</v>
       </c>
       <c r="AJ55" s="1">
-        <v>3010485.0</v>
+        <v>2781224.0</v>
       </c>
       <c r="AK55" s="2"/>
       <c r="AL55" s="1">
@@ -35606,7 +35536,7 @@
       <c r="E56" s="6"/>
       <c r="F56" s="2"/>
       <c r="G56" s="1">
-        <v>149620.0</v>
+        <v>244923.0</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
@@ -35648,10 +35578,10 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
       <c r="AI56" s="7">
-        <v>1210560.0</v>
+        <v>1115257.0</v>
       </c>
       <c r="AJ56" s="1">
-        <v>4221045.0</v>
+        <v>3896481.0</v>
       </c>
       <c r="AK56" s="2"/>
       <c r="AL56" s="1">
@@ -35683,7 +35613,7 @@
       <c r="E57" s="16"/>
       <c r="F57" s="17"/>
       <c r="G57" s="16">
-        <v>164582.0</v>
+        <v>276887.0</v>
       </c>
       <c r="H57" s="17">
         <v>0</v>
@@ -35725,10 +35655,10 @@
       <c r="AG57" s="17"/>
       <c r="AH57" s="17"/>
       <c r="AI57" s="16">
-        <v>1331616.0</v>
+        <v>1219311.0</v>
       </c>
       <c r="AJ57" s="16">
-        <v>5552661.0</v>
+        <v>5115792.0</v>
       </c>
       <c r="AK57" s="17"/>
       <c r="AL57" s="16">
@@ -35760,7 +35690,7 @@
       <c r="E58" s="6"/>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
-        <v>181040.0</v>
+        <v>312049.0</v>
       </c>
       <c r="H58" s="2">
         <v>0</v>
@@ -35802,10 +35732,10 @@
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="7">
-        <v>1464778.0</v>
+        <v>1333769.0</v>
       </c>
       <c r="AJ58" s="1">
-        <v>7017439.0</v>
+        <v>6449561.0</v>
       </c>
       <c r="AK58" s="2"/>
       <c r="AL58" s="1">
@@ -35837,7 +35767,7 @@
       <c r="E59" s="6"/>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
-        <v>199144.0</v>
+        <v>350725.0</v>
       </c>
       <c r="H59" s="2">
         <v>0</v>
@@ -35879,10 +35809,10 @@
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
       <c r="AI59" s="7">
-        <v>1611256.0</v>
+        <v>1459675.0</v>
       </c>
       <c r="AJ59" s="1">
-        <v>8628695.0</v>
+        <v>7909236.0</v>
       </c>
       <c r="AK59" s="2"/>
       <c r="AL59" s="1">
@@ -35914,7 +35844,7 @@
       <c r="E60" s="6"/>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
-        <v>219058.0</v>
+        <v>395003.0</v>
       </c>
       <c r="H60" s="2">
         <v>0</v>
@@ -35956,10 +35886,10 @@
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="7">
-        <v>1772382.0</v>
+        <v>1596437.0</v>
       </c>
       <c r="AJ60" s="1">
-        <v>10401077.0</v>
+        <v>9505673.0</v>
       </c>
       <c r="AK60" s="2"/>
       <c r="AL60" s="1">
@@ -35991,7 +35921,7 @@
       <c r="E61" s="6"/>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
-        <v>240964.0</v>
+        <v>444789.0</v>
       </c>
       <c r="H61" s="2">
         <v>0</v>
@@ -36033,10 +35963,10 @@
       <c r="AG61" s="2"/>
       <c r="AH61" s="2"/>
       <c r="AI61" s="7">
-        <v>1949620.0</v>
+        <v>1745795.0</v>
       </c>
       <c r="AJ61" s="1">
-        <v>12350697.0</v>
+        <v>11251468.0</v>
       </c>
       <c r="AK61" s="2"/>
       <c r="AL61" s="1">
@@ -36068,7 +35998,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
-        <v>265061.0</v>
+        <v>499555.0</v>
       </c>
       <c r="H62" s="2">
         <v>0</v>
@@ -36110,10 +36040,10 @@
       <c r="AG62" s="2"/>
       <c r="AH62" s="2"/>
       <c r="AI62" s="7">
-        <v>2144581.0</v>
+        <v>1910087.0</v>
       </c>
       <c r="AJ62" s="1">
-        <v>14495278.0</v>
+        <v>13161555.0</v>
       </c>
       <c r="AK62" s="2"/>
       <c r="AL62" s="1">
@@ -36145,7 +36075,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
-        <v>291567.0</v>
+        <v>559796.0</v>
       </c>
       <c r="H63" s="2">
         <v>0</v>
@@ -36187,10 +36117,10 @@
       <c r="AG63" s="2"/>
       <c r="AH63" s="2"/>
       <c r="AI63" s="7">
-        <v>2359039.0</v>
+        <v>2090810.0</v>
       </c>
       <c r="AJ63" s="1">
-        <v>16854317.0</v>
+        <v>15252365.0</v>
       </c>
       <c r="AK63" s="2"/>
       <c r="AL63" s="1">
@@ -36222,7 +36152,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
-        <v>320723.0</v>
+        <v>627139.0</v>
       </c>
       <c r="H64" s="2">
         <v>0</v>
@@ -36264,10 +36194,10 @@
       <c r="AG64" s="2"/>
       <c r="AH64" s="2"/>
       <c r="AI64" s="7">
-        <v>2594943.0</v>
+        <v>2288527.0</v>
       </c>
       <c r="AJ64" s="1">
-        <v>19449260.0</v>
+        <v>17540892.0</v>
       </c>
       <c r="AK64" s="2"/>
       <c r="AL64" s="1">
@@ -36299,7 +36229,7 @@
       <c r="E65" s="6"/>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
-        <v>352796.0</v>
+        <v>701489.0</v>
       </c>
       <c r="H65" s="2">
         <v>0</v>
@@ -36341,10 +36271,10 @@
       <c r="AG65" s="2"/>
       <c r="AH65" s="2"/>
       <c r="AI65" s="7">
-        <v>2854438.0</v>
+        <v>2505745.0</v>
       </c>
       <c r="AJ65" s="1">
-        <v>22303698.0</v>
+        <v>20046637.0</v>
       </c>
       <c r="AK65" s="2"/>
       <c r="AL65" s="1">
@@ -36376,7 +36306,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
-        <v>388075.0</v>
+        <v>783273.0</v>
       </c>
       <c r="H66" s="2">
         <v>0</v>
@@ -36418,10 +36348,10 @@
       <c r="AG66" s="2"/>
       <c r="AH66" s="2"/>
       <c r="AI66" s="7">
-        <v>3139883.0</v>
+        <v>2744685.0</v>
       </c>
       <c r="AJ66" s="1">
-        <v>25443581.0</v>
+        <v>22791322.0</v>
       </c>
       <c r="AK66" s="2"/>
       <c r="AL66" s="1">
@@ -36453,7 +36383,7 @@
       <c r="E67" s="6"/>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
-        <v>426883.0</v>
+        <v>873236.0</v>
       </c>
       <c r="H67" s="2">
         <v>0</v>
@@ -36495,10 +36425,10 @@
       <c r="AG67" s="2"/>
       <c r="AH67" s="2"/>
       <c r="AI67" s="7">
-        <v>3453869.0</v>
+        <v>3007516.0</v>
       </c>
       <c r="AJ67" s="1">
-        <v>28897450.0</v>
+        <v>25798838.0</v>
       </c>
       <c r="AK67" s="2"/>
       <c r="AL67" s="1">
@@ -36530,7 +36460,7 @@
       <c r="E68" s="6"/>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
-        <v>469571.0</v>
+        <v>972195.0</v>
       </c>
       <c r="H68" s="2">
         <v>0</v>
@@ -36572,10 +36502,10 @@
       <c r="AG68" s="2"/>
       <c r="AH68" s="2"/>
       <c r="AI68" s="7">
-        <v>3799257.0</v>
+        <v>3296633.0</v>
       </c>
       <c r="AJ68" s="1">
-        <v>32696707.0</v>
+        <v>29095471.0</v>
       </c>
       <c r="AK68" s="2"/>
       <c r="AL68" s="1">
@@ -36607,7 +36537,7 @@
       <c r="E69" s="6"/>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
-        <v>516528.0</v>
+        <v>1081051.0</v>
       </c>
       <c r="H69" s="2">
         <v>0</v>
@@ -36649,10 +36579,10 @@
       <c r="AG69" s="2"/>
       <c r="AH69" s="2"/>
       <c r="AI69" s="7">
-        <v>4179184.0</v>
+        <v>3614661.0</v>
       </c>
       <c r="AJ69" s="1">
-        <v>36875891.0</v>
+        <v>32710132.0</v>
       </c>
       <c r="AK69" s="2"/>
       <c r="AL69" s="1">
@@ -36684,7 +36614,7 @@
       <c r="E70" s="6"/>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
-        <v>568181.0</v>
+        <v>1200791.0</v>
       </c>
       <c r="H70" s="2">
         <v>0</v>
@@ -36726,10 +36656,10 @@
       <c r="AG70" s="2"/>
       <c r="AH70" s="2"/>
       <c r="AI70" s="7">
-        <v>4597101.0</v>
+        <v>3964491.0</v>
       </c>
       <c r="AJ70" s="1">
-        <v>41472992.0</v>
+        <v>36674623.0</v>
       </c>
       <c r="AK70" s="2"/>
       <c r="AL70" s="1">
@@ -36761,7 +36691,7 @@
       <c r="E71" s="6"/>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
-        <v>624999.0</v>
+        <v>1332505.0</v>
       </c>
       <c r="H71" s="2">
         <v>0</v>
@@ -36803,10 +36733,10 @@
       <c r="AG71" s="2"/>
       <c r="AH71" s="2"/>
       <c r="AI71" s="7">
-        <v>5056811.0</v>
+        <v>4349305.0</v>
       </c>
       <c r="AJ71" s="1">
-        <v>46529803.0</v>
+        <v>41023928.0</v>
       </c>
       <c r="AK71" s="2"/>
       <c r="AL71" s="1">
@@ -36838,7 +36768,7 @@
       <c r="E72" s="6"/>
       <c r="F72" s="20"/>
       <c r="G72" s="6">
-        <v>687499.0</v>
+        <v>1477392.0</v>
       </c>
       <c r="H72" s="20">
         <v>0</v>
@@ -36880,10 +36810,10 @@
       <c r="AG72" s="20"/>
       <c r="AH72" s="20"/>
       <c r="AI72" s="6">
-        <v>5562493.0</v>
+        <v>4772600.0</v>
       </c>
       <c r="AJ72" s="6">
-        <v>52092296.0</v>
+        <v>45796528.0</v>
       </c>
       <c r="AK72" s="20"/>
       <c r="AL72" s="6">

</xml_diff>